<commit_message>
Commit 30/09/2023 TestOps TestCloudRunTestListe Linux OS
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject\ANEF-AutomatizationProject\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC4A5B-D825-4152-A6EE-C016CD33889A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A1D716-A525-4DD4-A570-2AC1CF7A2017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -946,24 +946,24 @@
   <dimension ref="A1:J292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="75.54296875" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="45.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="75.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" customWidth="1"/>
     <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.81640625" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -995,7 +995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="11">
-        <v>7703039850</v>
+        <v>7703039863</v>
       </c>
       <c r="F2" s="20" t="s">
         <v>68</v>
@@ -1027,7 +1027,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="11">
-        <v>7703039851</v>
+        <v>7703039862</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>68</v>
@@ -1059,7 +1059,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="11">
-        <v>7703039852</v>
+        <v>7703039861</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>68</v>
@@ -1091,7 +1091,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>2</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>2</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>2</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>2</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>2</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>2</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>2</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>2</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B191" s="15"/>
       <c r="C191" s="15"/>
       <c r="D191" s="16"/>
@@ -1778,7 +1778,7 @@
       <c r="I191" s="16"/>
       <c r="J191" s="15"/>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>2</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>2</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>2</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>2</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>2</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>2</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>2</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>2</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>2</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>2</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>2</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>2</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>2</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>2</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>2</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>2</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>2</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>2</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>2</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>2</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>2</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>2</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>2</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>2</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>2</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>2</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>2</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>2</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>2</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>2</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>2</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>2</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>2</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="292" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Commit TestOps TestCloudRunTestListe Linux Os
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A1D716-A525-4DD4-A570-2AC1CF7A2017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0701F-4596-4250-A67D-5C82C2041C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$292</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$290</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="65">
   <si>
     <t>Usager</t>
   </si>
@@ -225,21 +225,6 @@
   </si>
   <si>
     <t>2 rue des 3 moulins 77000 melun</t>
-  </si>
-  <si>
-    <t>0911223346</t>
-  </si>
-  <si>
-    <t>0911223347</t>
-  </si>
-  <si>
-    <t>1PMTYE991215114515JY07</t>
-  </si>
-  <si>
-    <t>1PMTYE991215114515JY08</t>
-  </si>
-  <si>
-    <t>TS-PT-SalariéQualifié</t>
   </si>
   <si>
     <t>Profiles</t>
@@ -530,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -581,9 +566,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J292"/>
+  <dimension ref="A1:J290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,8 +938,8 @@
     <col min="3" max="3" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="24" customWidth="1"/>
     <col min="8" max="8" width="45.28515625" customWidth="1"/>
     <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" customWidth="1"/>
@@ -965,7 +947,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>54</v>
@@ -979,10 +961,10 @@
       <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -995,7 +977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1009,13 +991,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="11">
-        <v>7703039863</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>69</v>
+        <v>7703039864</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>61</v>
@@ -1027,68 +1009,56 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="11">
-        <v>7703039862</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11">
-        <v>7703039861</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>65</v>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="5"/>
+      <c r="D163" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E163" s="12">
+        <v>7703039343</v>
+      </c>
+      <c r="F163" s="21"/>
+      <c r="G163" s="21"/>
+      <c r="H163" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I163" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J163" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>2</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C164" s="5"/>
+      <c r="D164" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E164" s="12">
+        <v>7703039344</v>
+      </c>
+      <c r="F164" s="21"/>
+      <c r="G164" s="21"/>
+      <c r="H164" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I164" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,12 +1073,12 @@
         <v>2</v>
       </c>
       <c r="E165" s="12">
-        <v>7703039343</v>
-      </c>
-      <c r="F165" s="22"/>
-      <c r="G165" s="22"/>
+        <v>7703039345</v>
+      </c>
+      <c r="F165" s="21"/>
+      <c r="G165" s="21"/>
       <c r="H165" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I165" s="6" t="s">
         <v>45</v>
@@ -1129,12 +1099,12 @@
         <v>2</v>
       </c>
       <c r="E166" s="12">
-        <v>7703039344</v>
-      </c>
-      <c r="F166" s="22"/>
-      <c r="G166" s="22"/>
+        <v>7703039346</v>
+      </c>
+      <c r="F166" s="21"/>
+      <c r="G166" s="21"/>
       <c r="H166" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I166" s="6" t="s">
         <v>45</v>
@@ -1155,12 +1125,12 @@
         <v>2</v>
       </c>
       <c r="E167" s="12">
-        <v>7703039345</v>
-      </c>
-      <c r="F167" s="22"/>
-      <c r="G167" s="22"/>
+        <v>7703039347</v>
+      </c>
+      <c r="F167" s="21"/>
+      <c r="G167" s="21"/>
       <c r="H167" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I167" s="6" t="s">
         <v>45</v>
@@ -1181,12 +1151,12 @@
         <v>2</v>
       </c>
       <c r="E168" s="12">
-        <v>7703039346</v>
-      </c>
-      <c r="F168" s="22"/>
-      <c r="G168" s="22"/>
+        <v>7703039348</v>
+      </c>
+      <c r="F168" s="21"/>
+      <c r="G168" s="21"/>
       <c r="H168" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I168" s="6" t="s">
         <v>45</v>
@@ -1207,12 +1177,12 @@
         <v>2</v>
       </c>
       <c r="E169" s="12">
-        <v>7703039347</v>
-      </c>
-      <c r="F169" s="22"/>
-      <c r="G169" s="22"/>
+        <v>7703039349</v>
+      </c>
+      <c r="F169" s="21"/>
+      <c r="G169" s="21"/>
       <c r="H169" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I169" s="6" t="s">
         <v>45</v>
@@ -1233,12 +1203,12 @@
         <v>2</v>
       </c>
       <c r="E170" s="12">
-        <v>7703039348</v>
-      </c>
-      <c r="F170" s="22"/>
-      <c r="G170" s="22"/>
+        <v>7703039350</v>
+      </c>
+      <c r="F170" s="21"/>
+      <c r="G170" s="21"/>
       <c r="H170" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I170" s="6" t="s">
         <v>45</v>
@@ -1259,12 +1229,12 @@
         <v>2</v>
       </c>
       <c r="E171" s="12">
-        <v>7703039349</v>
-      </c>
-      <c r="F171" s="22"/>
-      <c r="G171" s="22"/>
+        <v>7703039351</v>
+      </c>
+      <c r="F171" s="21"/>
+      <c r="G171" s="21"/>
       <c r="H171" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I171" s="6" t="s">
         <v>45</v>
@@ -1285,12 +1255,12 @@
         <v>2</v>
       </c>
       <c r="E172" s="12">
-        <v>7703039350</v>
-      </c>
-      <c r="F172" s="22"/>
-      <c r="G172" s="22"/>
+        <v>7703039352</v>
+      </c>
+      <c r="F172" s="21"/>
+      <c r="G172" s="21"/>
       <c r="H172" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I172" s="6" t="s">
         <v>45</v>
@@ -1311,12 +1281,12 @@
         <v>2</v>
       </c>
       <c r="E173" s="12">
-        <v>7703039351</v>
-      </c>
-      <c r="F173" s="22"/>
-      <c r="G173" s="22"/>
+        <v>7703039353</v>
+      </c>
+      <c r="F173" s="21"/>
+      <c r="G173" s="21"/>
       <c r="H173" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I173" s="6" t="s">
         <v>45</v>
@@ -1337,12 +1307,12 @@
         <v>2</v>
       </c>
       <c r="E174" s="12">
-        <v>7703039352</v>
-      </c>
-      <c r="F174" s="22"/>
-      <c r="G174" s="22"/>
+        <v>7703039354</v>
+      </c>
+      <c r="F174" s="21"/>
+      <c r="G174" s="21"/>
       <c r="H174" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I174" s="6" t="s">
         <v>45</v>
@@ -1363,12 +1333,12 @@
         <v>2</v>
       </c>
       <c r="E175" s="12">
-        <v>7703039353</v>
-      </c>
-      <c r="F175" s="22"/>
-      <c r="G175" s="22"/>
+        <v>7703039355</v>
+      </c>
+      <c r="F175" s="21"/>
+      <c r="G175" s="21"/>
       <c r="H175" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I175" s="6" t="s">
         <v>45</v>
@@ -1389,12 +1359,12 @@
         <v>2</v>
       </c>
       <c r="E176" s="12">
-        <v>7703039354</v>
-      </c>
-      <c r="F176" s="22"/>
-      <c r="G176" s="22"/>
+        <v>7703039356</v>
+      </c>
+      <c r="F176" s="21"/>
+      <c r="G176" s="21"/>
       <c r="H176" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I176" s="6" t="s">
         <v>45</v>
@@ -1415,12 +1385,12 @@
         <v>2</v>
       </c>
       <c r="E177" s="12">
-        <v>7703039355</v>
-      </c>
-      <c r="F177" s="22"/>
-      <c r="G177" s="22"/>
+        <v>7703039357</v>
+      </c>
+      <c r="F177" s="21"/>
+      <c r="G177" s="21"/>
       <c r="H177" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I177" s="6" t="s">
         <v>45</v>
@@ -1441,12 +1411,12 @@
         <v>2</v>
       </c>
       <c r="E178" s="12">
-        <v>7703039356</v>
-      </c>
-      <c r="F178" s="22"/>
-      <c r="G178" s="22"/>
+        <v>7703039358</v>
+      </c>
+      <c r="F178" s="21"/>
+      <c r="G178" s="21"/>
       <c r="H178" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I178" s="6" t="s">
         <v>45</v>
@@ -1467,12 +1437,12 @@
         <v>2</v>
       </c>
       <c r="E179" s="12">
-        <v>7703039357</v>
-      </c>
-      <c r="F179" s="22"/>
-      <c r="G179" s="22"/>
+        <v>7703039359</v>
+      </c>
+      <c r="F179" s="21"/>
+      <c r="G179" s="21"/>
       <c r="H179" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I179" s="6" t="s">
         <v>45</v>
@@ -1493,12 +1463,12 @@
         <v>2</v>
       </c>
       <c r="E180" s="12">
-        <v>7703039358</v>
-      </c>
-      <c r="F180" s="22"/>
-      <c r="G180" s="22"/>
+        <v>7703039360</v>
+      </c>
+      <c r="F180" s="21"/>
+      <c r="G180" s="21"/>
       <c r="H180" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I180" s="6" t="s">
         <v>45</v>
@@ -1519,12 +1489,12 @@
         <v>2</v>
       </c>
       <c r="E181" s="12">
-        <v>7703039359</v>
-      </c>
-      <c r="F181" s="22"/>
-      <c r="G181" s="22"/>
+        <v>7703039361</v>
+      </c>
+      <c r="F181" s="21"/>
+      <c r="G181" s="21"/>
       <c r="H181" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I181" s="6" t="s">
         <v>45</v>
@@ -1545,12 +1515,12 @@
         <v>2</v>
       </c>
       <c r="E182" s="12">
-        <v>7703039360</v>
-      </c>
-      <c r="F182" s="22"/>
-      <c r="G182" s="22"/>
+        <v>7703039362</v>
+      </c>
+      <c r="F182" s="21"/>
+      <c r="G182" s="21"/>
       <c r="H182" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I182" s="6" t="s">
         <v>45</v>
@@ -1571,12 +1541,12 @@
         <v>2</v>
       </c>
       <c r="E183" s="12">
-        <v>7703039361</v>
-      </c>
-      <c r="F183" s="22"/>
-      <c r="G183" s="22"/>
+        <v>7703039363</v>
+      </c>
+      <c r="F183" s="21"/>
+      <c r="G183" s="21"/>
       <c r="H183" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I183" s="6" t="s">
         <v>45</v>
@@ -1597,12 +1567,12 @@
         <v>2</v>
       </c>
       <c r="E184" s="12">
-        <v>7703039362</v>
-      </c>
-      <c r="F184" s="22"/>
-      <c r="G184" s="22"/>
+        <v>7703039364</v>
+      </c>
+      <c r="F184" s="21"/>
+      <c r="G184" s="21"/>
       <c r="H184" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I184" s="6" t="s">
         <v>45</v>
@@ -1623,12 +1593,12 @@
         <v>2</v>
       </c>
       <c r="E185" s="12">
-        <v>7703039363</v>
-      </c>
-      <c r="F185" s="22"/>
-      <c r="G185" s="22"/>
+        <v>7703039365</v>
+      </c>
+      <c r="F185" s="21"/>
+      <c r="G185" s="21"/>
       <c r="H185" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I185" s="6" t="s">
         <v>45</v>
@@ -1649,12 +1619,12 @@
         <v>2</v>
       </c>
       <c r="E186" s="12">
-        <v>7703039364</v>
-      </c>
-      <c r="F186" s="22"/>
-      <c r="G186" s="22"/>
+        <v>7703039366</v>
+      </c>
+      <c r="F186" s="21"/>
+      <c r="G186" s="21"/>
       <c r="H186" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I186" s="6" t="s">
         <v>45</v>
@@ -1675,12 +1645,12 @@
         <v>2</v>
       </c>
       <c r="E187" s="12">
-        <v>7703039365</v>
-      </c>
-      <c r="F187" s="22"/>
-      <c r="G187" s="22"/>
+        <v>7703039367</v>
+      </c>
+      <c r="F187" s="21"/>
+      <c r="G187" s="21"/>
       <c r="H187" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I187" s="6" t="s">
         <v>45</v>
@@ -1701,12 +1671,12 @@
         <v>2</v>
       </c>
       <c r="E188" s="12">
-        <v>7703039366</v>
-      </c>
-      <c r="F188" s="22"/>
-      <c r="G188" s="22"/>
+        <v>7703039368</v>
+      </c>
+      <c r="F188" s="21"/>
+      <c r="G188" s="21"/>
       <c r="H188" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I188" s="6" t="s">
         <v>45</v>
@@ -1716,67 +1686,67 @@
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>2</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C189" s="5"/>
-      <c r="D189" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E189" s="12">
-        <v>7703039367</v>
-      </c>
+      <c r="B189" s="15"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="16"/>
+      <c r="E189" s="14"/>
       <c r="F189" s="22"/>
       <c r="G189" s="22"/>
-      <c r="H189" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I189" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J189" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>2</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C190" s="5"/>
-      <c r="D190" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E190" s="12">
-        <v>7703039368</v>
-      </c>
-      <c r="F190" s="22"/>
-      <c r="G190" s="22"/>
-      <c r="H190" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I190" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J190" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B191" s="15"/>
-      <c r="C191" s="15"/>
-      <c r="D191" s="16"/>
-      <c r="E191" s="14"/>
-      <c r="F191" s="23"/>
-      <c r="G191" s="23"/>
-      <c r="H191" s="15"/>
-      <c r="I191" s="16"/>
-      <c r="J191" s="15"/>
+      <c r="H189" s="15"/>
+      <c r="I189" s="16"/>
+      <c r="J189" s="15"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>2</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C251" s="5"/>
+      <c r="D251" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E251" s="12">
+        <v>7703039429</v>
+      </c>
+      <c r="F251" s="21"/>
+      <c r="G251" s="21"/>
+      <c r="H251" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I251" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J251" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>2</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C252" s="5"/>
+      <c r="D252" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E252" s="12">
+        <v>7703039430</v>
+      </c>
+      <c r="F252" s="21"/>
+      <c r="G252" s="21"/>
+      <c r="H252" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I252" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J252" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
@@ -1790,12 +1760,12 @@
         <v>2</v>
       </c>
       <c r="E253" s="12">
-        <v>7703039429</v>
-      </c>
-      <c r="F253" s="22"/>
-      <c r="G253" s="22"/>
+        <v>7703039431</v>
+      </c>
+      <c r="F253" s="21"/>
+      <c r="G253" s="21"/>
       <c r="H253" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I253" s="6" t="s">
         <v>47</v>
@@ -1816,12 +1786,12 @@
         <v>2</v>
       </c>
       <c r="E254" s="12">
-        <v>7703039430</v>
-      </c>
-      <c r="F254" s="22"/>
-      <c r="G254" s="22"/>
+        <v>7703039432</v>
+      </c>
+      <c r="F254" s="21"/>
+      <c r="G254" s="21"/>
       <c r="H254" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I254" s="6" t="s">
         <v>47</v>
@@ -1842,12 +1812,12 @@
         <v>2</v>
       </c>
       <c r="E255" s="12">
-        <v>7703039431</v>
-      </c>
-      <c r="F255" s="22"/>
-      <c r="G255" s="22"/>
+        <v>7703039433</v>
+      </c>
+      <c r="F255" s="21"/>
+      <c r="G255" s="21"/>
       <c r="H255" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I255" s="6" t="s">
         <v>47</v>
@@ -1868,12 +1838,12 @@
         <v>2</v>
       </c>
       <c r="E256" s="12">
-        <v>7703039432</v>
-      </c>
-      <c r="F256" s="22"/>
-      <c r="G256" s="22"/>
+        <v>7703039434</v>
+      </c>
+      <c r="F256" s="21"/>
+      <c r="G256" s="21"/>
       <c r="H256" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I256" s="6" t="s">
         <v>47</v>
@@ -1894,12 +1864,12 @@
         <v>2</v>
       </c>
       <c r="E257" s="12">
-        <v>7703039433</v>
-      </c>
-      <c r="F257" s="22"/>
-      <c r="G257" s="22"/>
+        <v>7703039435</v>
+      </c>
+      <c r="F257" s="21"/>
+      <c r="G257" s="21"/>
       <c r="H257" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I257" s="6" t="s">
         <v>47</v>
@@ -1920,12 +1890,12 @@
         <v>2</v>
       </c>
       <c r="E258" s="12">
-        <v>7703039434</v>
-      </c>
-      <c r="F258" s="22"/>
-      <c r="G258" s="22"/>
+        <v>7703039436</v>
+      </c>
+      <c r="F258" s="21"/>
+      <c r="G258" s="21"/>
       <c r="H258" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I258" s="6" t="s">
         <v>47</v>
@@ -1946,12 +1916,12 @@
         <v>2</v>
       </c>
       <c r="E259" s="12">
-        <v>7703039435</v>
-      </c>
-      <c r="F259" s="22"/>
-      <c r="G259" s="22"/>
+        <v>7703039437</v>
+      </c>
+      <c r="F259" s="21"/>
+      <c r="G259" s="21"/>
       <c r="H259" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I259" s="6" t="s">
         <v>47</v>
@@ -1972,12 +1942,12 @@
         <v>2</v>
       </c>
       <c r="E260" s="12">
-        <v>7703039436</v>
-      </c>
-      <c r="F260" s="22"/>
-      <c r="G260" s="22"/>
+        <v>7703039438</v>
+      </c>
+      <c r="F260" s="21"/>
+      <c r="G260" s="21"/>
       <c r="H260" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I260" s="6" t="s">
         <v>47</v>
@@ -1998,12 +1968,12 @@
         <v>2</v>
       </c>
       <c r="E261" s="12">
-        <v>7703039437</v>
-      </c>
-      <c r="F261" s="22"/>
-      <c r="G261" s="22"/>
+        <v>7703039439</v>
+      </c>
+      <c r="F261" s="21"/>
+      <c r="G261" s="21"/>
       <c r="H261" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I261" s="6" t="s">
         <v>47</v>
@@ -2024,12 +1994,12 @@
         <v>2</v>
       </c>
       <c r="E262" s="12">
-        <v>7703039438</v>
-      </c>
-      <c r="F262" s="22"/>
-      <c r="G262" s="22"/>
+        <v>7703039440</v>
+      </c>
+      <c r="F262" s="21"/>
+      <c r="G262" s="21"/>
       <c r="H262" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I262" s="6" t="s">
         <v>47</v>
@@ -2050,12 +2020,12 @@
         <v>2</v>
       </c>
       <c r="E263" s="12">
-        <v>7703039439</v>
-      </c>
-      <c r="F263" s="22"/>
-      <c r="G263" s="22"/>
+        <v>7703039441</v>
+      </c>
+      <c r="F263" s="21"/>
+      <c r="G263" s="21"/>
       <c r="H263" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I263" s="6" t="s">
         <v>47</v>
@@ -2076,12 +2046,12 @@
         <v>2</v>
       </c>
       <c r="E264" s="12">
-        <v>7703039440</v>
-      </c>
-      <c r="F264" s="22"/>
-      <c r="G264" s="22"/>
+        <v>7703039442</v>
+      </c>
+      <c r="F264" s="21"/>
+      <c r="G264" s="21"/>
       <c r="H264" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I264" s="6" t="s">
         <v>47</v>
@@ -2102,12 +2072,12 @@
         <v>2</v>
       </c>
       <c r="E265" s="12">
-        <v>7703039441</v>
-      </c>
-      <c r="F265" s="22"/>
-      <c r="G265" s="22"/>
+        <v>7703039443</v>
+      </c>
+      <c r="F265" s="21"/>
+      <c r="G265" s="21"/>
       <c r="H265" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I265" s="6" t="s">
         <v>47</v>
@@ -2128,12 +2098,12 @@
         <v>2</v>
       </c>
       <c r="E266" s="12">
-        <v>7703039442</v>
-      </c>
-      <c r="F266" s="22"/>
-      <c r="G266" s="22"/>
+        <v>7703039444</v>
+      </c>
+      <c r="F266" s="21"/>
+      <c r="G266" s="21"/>
       <c r="H266" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I266" s="6" t="s">
         <v>47</v>
@@ -2154,12 +2124,12 @@
         <v>2</v>
       </c>
       <c r="E267" s="12">
-        <v>7703039443</v>
-      </c>
-      <c r="F267" s="22"/>
-      <c r="G267" s="22"/>
+        <v>7703039445</v>
+      </c>
+      <c r="F267" s="21"/>
+      <c r="G267" s="21"/>
       <c r="H267" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I267" s="6" t="s">
         <v>47</v>
@@ -2180,12 +2150,12 @@
         <v>2</v>
       </c>
       <c r="E268" s="12">
-        <v>7703039444</v>
-      </c>
-      <c r="F268" s="22"/>
-      <c r="G268" s="22"/>
+        <v>7703039446</v>
+      </c>
+      <c r="F268" s="21"/>
+      <c r="G268" s="21"/>
       <c r="H268" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I268" s="6" t="s">
         <v>47</v>
@@ -2206,12 +2176,12 @@
         <v>2</v>
       </c>
       <c r="E269" s="12">
-        <v>7703039445</v>
-      </c>
-      <c r="F269" s="22"/>
-      <c r="G269" s="22"/>
+        <v>7703039447</v>
+      </c>
+      <c r="F269" s="21"/>
+      <c r="G269" s="21"/>
       <c r="H269" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I269" s="6" t="s">
         <v>47</v>
@@ -2232,12 +2202,12 @@
         <v>2</v>
       </c>
       <c r="E270" s="12">
-        <v>7703039446</v>
-      </c>
-      <c r="F270" s="22"/>
-      <c r="G270" s="22"/>
+        <v>7703039448</v>
+      </c>
+      <c r="F270" s="21"/>
+      <c r="G270" s="21"/>
       <c r="H270" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I270" s="6" t="s">
         <v>47</v>
@@ -2258,12 +2228,12 @@
         <v>2</v>
       </c>
       <c r="E271" s="12">
-        <v>7703039447</v>
-      </c>
-      <c r="F271" s="22"/>
-      <c r="G271" s="22"/>
+        <v>7703039449</v>
+      </c>
+      <c r="F271" s="21"/>
+      <c r="G271" s="21"/>
       <c r="H271" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I271" s="6" t="s">
         <v>47</v>
@@ -2284,12 +2254,12 @@
         <v>2</v>
       </c>
       <c r="E272" s="12">
-        <v>7703039448</v>
-      </c>
-      <c r="F272" s="22"/>
-      <c r="G272" s="22"/>
+        <v>7703039450</v>
+      </c>
+      <c r="F272" s="21"/>
+      <c r="G272" s="21"/>
       <c r="H272" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I272" s="6" t="s">
         <v>47</v>
@@ -2310,12 +2280,12 @@
         <v>2</v>
       </c>
       <c r="E273" s="12">
-        <v>7703039449</v>
-      </c>
-      <c r="F273" s="22"/>
-      <c r="G273" s="22"/>
+        <v>7703039451</v>
+      </c>
+      <c r="F273" s="21"/>
+      <c r="G273" s="21"/>
       <c r="H273" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I273" s="6" t="s">
         <v>47</v>
@@ -2336,12 +2306,12 @@
         <v>2</v>
       </c>
       <c r="E274" s="12">
-        <v>7703039450</v>
-      </c>
-      <c r="F274" s="22"/>
-      <c r="G274" s="22"/>
+        <v>7703039452</v>
+      </c>
+      <c r="F274" s="21"/>
+      <c r="G274" s="21"/>
       <c r="H274" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I274" s="6" t="s">
         <v>47</v>
@@ -2362,12 +2332,12 @@
         <v>2</v>
       </c>
       <c r="E275" s="12">
-        <v>7703039451</v>
-      </c>
-      <c r="F275" s="22"/>
-      <c r="G275" s="22"/>
+        <v>7703039453</v>
+      </c>
+      <c r="F275" s="21"/>
+      <c r="G275" s="21"/>
       <c r="H275" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I275" s="6" t="s">
         <v>47</v>
@@ -2388,12 +2358,12 @@
         <v>2</v>
       </c>
       <c r="E276" s="12">
-        <v>7703039452</v>
-      </c>
-      <c r="F276" s="22"/>
-      <c r="G276" s="22"/>
+        <v>7703039454</v>
+      </c>
+      <c r="F276" s="21"/>
+      <c r="G276" s="21"/>
       <c r="H276" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I276" s="6" t="s">
         <v>47</v>
@@ -2414,12 +2384,12 @@
         <v>2</v>
       </c>
       <c r="E277" s="12">
-        <v>7703039453</v>
-      </c>
-      <c r="F277" s="22"/>
-      <c r="G277" s="22"/>
+        <v>7703039455</v>
+      </c>
+      <c r="F277" s="21"/>
+      <c r="G277" s="21"/>
       <c r="H277" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I277" s="6" t="s">
         <v>47</v>
@@ -2440,12 +2410,12 @@
         <v>2</v>
       </c>
       <c r="E278" s="12">
-        <v>7703039454</v>
-      </c>
-      <c r="F278" s="22"/>
-      <c r="G278" s="22"/>
+        <v>7703039456</v>
+      </c>
+      <c r="F278" s="21"/>
+      <c r="G278" s="21"/>
       <c r="H278" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I278" s="6" t="s">
         <v>47</v>
@@ -2466,12 +2436,12 @@
         <v>2</v>
       </c>
       <c r="E279" s="12">
-        <v>7703039455</v>
-      </c>
-      <c r="F279" s="22"/>
-      <c r="G279" s="22"/>
+        <v>7703039457</v>
+      </c>
+      <c r="F279" s="21"/>
+      <c r="G279" s="21"/>
       <c r="H279" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I279" s="6" t="s">
         <v>47</v>
@@ -2492,12 +2462,12 @@
         <v>2</v>
       </c>
       <c r="E280" s="12">
-        <v>7703039456</v>
-      </c>
-      <c r="F280" s="22"/>
-      <c r="G280" s="22"/>
+        <v>7703039458</v>
+      </c>
+      <c r="F280" s="21"/>
+      <c r="G280" s="21"/>
       <c r="H280" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I280" s="6" t="s">
         <v>47</v>
@@ -2518,12 +2488,12 @@
         <v>2</v>
       </c>
       <c r="E281" s="12">
-        <v>7703039457</v>
-      </c>
-      <c r="F281" s="22"/>
-      <c r="G281" s="22"/>
+        <v>7703039459</v>
+      </c>
+      <c r="F281" s="21"/>
+      <c r="G281" s="21"/>
       <c r="H281" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I281" s="6" t="s">
         <v>47</v>
@@ -2544,12 +2514,12 @@
         <v>2</v>
       </c>
       <c r="E282" s="12">
-        <v>7703039458</v>
-      </c>
-      <c r="F282" s="22"/>
-      <c r="G282" s="22"/>
+        <v>7703039460</v>
+      </c>
+      <c r="F282" s="21"/>
+      <c r="G282" s="21"/>
       <c r="H282" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I282" s="6" t="s">
         <v>47</v>
@@ -2570,12 +2540,12 @@
         <v>2</v>
       </c>
       <c r="E283" s="12">
-        <v>7703039459</v>
-      </c>
-      <c r="F283" s="22"/>
-      <c r="G283" s="22"/>
+        <v>7703039461</v>
+      </c>
+      <c r="F283" s="21"/>
+      <c r="G283" s="21"/>
       <c r="H283" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I283" s="6" t="s">
         <v>47</v>
@@ -2596,12 +2566,12 @@
         <v>2</v>
       </c>
       <c r="E284" s="12">
-        <v>7703039460</v>
-      </c>
-      <c r="F284" s="22"/>
-      <c r="G284" s="22"/>
+        <v>7703039462</v>
+      </c>
+      <c r="F284" s="21"/>
+      <c r="G284" s="21"/>
       <c r="H284" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I284" s="6" t="s">
         <v>47</v>
@@ -2622,12 +2592,12 @@
         <v>2</v>
       </c>
       <c r="E285" s="12">
-        <v>7703039461</v>
-      </c>
-      <c r="F285" s="22"/>
-      <c r="G285" s="22"/>
+        <v>7703039463</v>
+      </c>
+      <c r="F285" s="21"/>
+      <c r="G285" s="21"/>
       <c r="H285" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I285" s="6" t="s">
         <v>47</v>
@@ -2648,12 +2618,12 @@
         <v>2</v>
       </c>
       <c r="E286" s="12">
-        <v>7703039462</v>
-      </c>
-      <c r="F286" s="22"/>
-      <c r="G286" s="22"/>
+        <v>7703039464</v>
+      </c>
+      <c r="F286" s="21"/>
+      <c r="G286" s="21"/>
       <c r="H286" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I286" s="6" t="s">
         <v>47</v>
@@ -2674,12 +2644,12 @@
         <v>2</v>
       </c>
       <c r="E287" s="12">
-        <v>7703039463</v>
-      </c>
-      <c r="F287" s="22"/>
-      <c r="G287" s="22"/>
+        <v>7703039465</v>
+      </c>
+      <c r="F287" s="21"/>
+      <c r="G287" s="21"/>
       <c r="H287" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I287" s="6" t="s">
         <v>47</v>
@@ -2700,12 +2670,12 @@
         <v>2</v>
       </c>
       <c r="E288" s="12">
-        <v>7703039464</v>
-      </c>
-      <c r="F288" s="22"/>
-      <c r="G288" s="22"/>
+        <v>7703039466</v>
+      </c>
+      <c r="F288" s="21"/>
+      <c r="G288" s="21"/>
       <c r="H288" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I288" s="6" t="s">
         <v>47</v>
@@ -2726,12 +2696,12 @@
         <v>2</v>
       </c>
       <c r="E289" s="12">
-        <v>7703039465</v>
-      </c>
-      <c r="F289" s="22"/>
-      <c r="G289" s="22"/>
+        <v>7703039467</v>
+      </c>
+      <c r="F289" s="21"/>
+      <c r="G289" s="21"/>
       <c r="H289" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I289" s="6" t="s">
         <v>47</v>
@@ -2740,81 +2710,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>2</v>
       </c>
-      <c r="B290" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C290" s="5"/>
-      <c r="D290" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E290" s="12">
-        <v>7703039466</v>
-      </c>
-      <c r="F290" s="22"/>
-      <c r="G290" s="22"/>
-      <c r="H290" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I290" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J290" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>2</v>
-      </c>
-      <c r="B291" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C291" s="5"/>
-      <c r="D291" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E291" s="12">
-        <v>7703039467</v>
-      </c>
-      <c r="F291" s="22"/>
-      <c r="G291" s="22"/>
-      <c r="H291" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I291" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J291" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="292" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" t="s">
-        <v>2</v>
-      </c>
-      <c r="B292" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C292" s="8"/>
-      <c r="D292" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E292" s="13">
+      <c r="B290" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C290" s="8"/>
+      <c r="D290" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E290" s="13">
         <v>7703039468</v>
       </c>
-      <c r="F292" s="24"/>
-      <c r="G292" s="24"/>
-      <c r="H292" s="8" t="s">
+      <c r="F290" s="23"/>
+      <c r="G290" s="23"/>
+      <c r="H290" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I292" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J292" s="8" t="s">
+      <c r="I290" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J290" s="8" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Titre De Séjour Visiteur + Renouvellement
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0701F-4596-4250-A67D-5C82C2041C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E750830-7B86-4B9F-B9F1-12EFA5048120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$290</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$288</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="64">
   <si>
     <t>Usager</t>
   </si>
   <si>
-    <t>Etudiant</t>
-  </si>
-  <si>
     <t>Visiteur</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>TypeTitreDeSejour</t>
   </si>
   <si>
-    <t>RenouvellementDeTitreSéjour</t>
-  </si>
-  <si>
     <t>0911223344</t>
   </si>
   <si>
@@ -234,6 +228,9 @@
   </si>
   <si>
     <t>30/11/2023</t>
+  </si>
+  <si>
+    <t>RenouvellementDeTitreSejour</t>
   </si>
 </sst>
 </file>
@@ -925,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J290"/>
+  <dimension ref="A1:J288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,1793 +944,1793 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>7703039887</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11">
-        <v>7703039864</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" s="5"/>
+      <c r="D161" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E161" s="12">
+        <v>7703039343</v>
+      </c>
+      <c r="F161" s="21"/>
+      <c r="G161" s="21"/>
+      <c r="H161" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I161" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J161" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C162" s="5"/>
+      <c r="D162" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E162" s="12">
+        <v>7703039344</v>
+      </c>
+      <c r="F162" s="21"/>
+      <c r="G162" s="21"/>
+      <c r="H162" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I162" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J162" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C163" s="5"/>
       <c r="D163" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E163" s="12">
-        <v>7703039343</v>
+        <v>7703039345</v>
       </c>
       <c r="F163" s="21"/>
       <c r="G163" s="21"/>
       <c r="H163" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I163" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J163" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J163" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E164" s="12">
-        <v>7703039344</v>
+        <v>7703039346</v>
       </c>
       <c r="F164" s="21"/>
       <c r="G164" s="21"/>
       <c r="H164" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I164" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J164" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J164" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C165" s="5"/>
       <c r="D165" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E165" s="12">
-        <v>7703039345</v>
+        <v>7703039347</v>
       </c>
       <c r="F165" s="21"/>
       <c r="G165" s="21"/>
       <c r="H165" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I165" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J165" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J165" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C166" s="5"/>
       <c r="D166" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E166" s="12">
-        <v>7703039346</v>
+        <v>7703039348</v>
       </c>
       <c r="F166" s="21"/>
       <c r="G166" s="21"/>
       <c r="H166" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I166" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J166" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J166" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C167" s="5"/>
       <c r="D167" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167" s="12">
-        <v>7703039347</v>
+        <v>7703039349</v>
       </c>
       <c r="F167" s="21"/>
       <c r="G167" s="21"/>
       <c r="H167" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I167" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J167" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J167" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C168" s="5"/>
       <c r="D168" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E168" s="12">
-        <v>7703039348</v>
+        <v>7703039350</v>
       </c>
       <c r="F168" s="21"/>
       <c r="G168" s="21"/>
       <c r="H168" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I168" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J168" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J168" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E169" s="12">
-        <v>7703039349</v>
+        <v>7703039351</v>
       </c>
       <c r="F169" s="21"/>
       <c r="G169" s="21"/>
       <c r="H169" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I169" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J169" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J169" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C170" s="5"/>
       <c r="D170" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E170" s="12">
-        <v>7703039350</v>
+        <v>7703039352</v>
       </c>
       <c r="F170" s="21"/>
       <c r="G170" s="21"/>
       <c r="H170" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I170" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J170" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J170" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C171" s="5"/>
       <c r="D171" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E171" s="12">
-        <v>7703039351</v>
+        <v>7703039353</v>
       </c>
       <c r="F171" s="21"/>
       <c r="G171" s="21"/>
       <c r="H171" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I171" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J171" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J171" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C172" s="5"/>
       <c r="D172" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E172" s="12">
-        <v>7703039352</v>
+        <v>7703039354</v>
       </c>
       <c r="F172" s="21"/>
       <c r="G172" s="21"/>
       <c r="H172" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I172" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J172" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J172" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173" s="5"/>
       <c r="D173" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E173" s="12">
-        <v>7703039353</v>
+        <v>7703039355</v>
       </c>
       <c r="F173" s="21"/>
       <c r="G173" s="21"/>
       <c r="H173" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I173" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J173" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J173" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E174" s="12">
-        <v>7703039354</v>
+        <v>7703039356</v>
       </c>
       <c r="F174" s="21"/>
       <c r="G174" s="21"/>
       <c r="H174" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I174" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J174" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J174" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E175" s="12">
-        <v>7703039355</v>
+        <v>7703039357</v>
       </c>
       <c r="F175" s="21"/>
       <c r="G175" s="21"/>
       <c r="H175" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I175" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J175" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J175" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C176" s="5"/>
       <c r="D176" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E176" s="12">
-        <v>7703039356</v>
+        <v>7703039358</v>
       </c>
       <c r="F176" s="21"/>
       <c r="G176" s="21"/>
       <c r="H176" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I176" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J176" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J176" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C177" s="5"/>
       <c r="D177" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E177" s="12">
-        <v>7703039357</v>
+        <v>7703039359</v>
       </c>
       <c r="F177" s="21"/>
       <c r="G177" s="21"/>
       <c r="H177" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I177" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J177" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J177" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C178" s="5"/>
       <c r="D178" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E178" s="12">
-        <v>7703039358</v>
+        <v>7703039360</v>
       </c>
       <c r="F178" s="21"/>
       <c r="G178" s="21"/>
       <c r="H178" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I178" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J178" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J178" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C179" s="5"/>
       <c r="D179" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E179" s="12">
-        <v>7703039359</v>
+        <v>7703039361</v>
       </c>
       <c r="F179" s="21"/>
       <c r="G179" s="21"/>
       <c r="H179" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I179" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J179" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J179" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C180" s="5"/>
       <c r="D180" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E180" s="12">
-        <v>7703039360</v>
+        <v>7703039362</v>
       </c>
       <c r="F180" s="21"/>
       <c r="G180" s="21"/>
       <c r="H180" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I180" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J180" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J180" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C181" s="5"/>
       <c r="D181" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E181" s="12">
-        <v>7703039361</v>
+        <v>7703039363</v>
       </c>
       <c r="F181" s="21"/>
       <c r="G181" s="21"/>
       <c r="H181" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I181" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J181" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J181" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C182" s="5"/>
       <c r="D182" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E182" s="12">
-        <v>7703039362</v>
+        <v>7703039364</v>
       </c>
       <c r="F182" s="21"/>
       <c r="G182" s="21"/>
       <c r="H182" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I182" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J182" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J182" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C183" s="5"/>
       <c r="D183" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E183" s="12">
-        <v>7703039363</v>
+        <v>7703039365</v>
       </c>
       <c r="F183" s="21"/>
       <c r="G183" s="21"/>
       <c r="H183" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I183" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J183" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J183" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C184" s="5"/>
       <c r="D184" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E184" s="12">
-        <v>7703039364</v>
+        <v>7703039366</v>
       </c>
       <c r="F184" s="21"/>
       <c r="G184" s="21"/>
       <c r="H184" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I184" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J184" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J184" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C185" s="5"/>
       <c r="D185" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E185" s="12">
-        <v>7703039365</v>
+        <v>7703039367</v>
       </c>
       <c r="F185" s="21"/>
       <c r="G185" s="21"/>
       <c r="H185" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I185" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J185" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="J185" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C186" s="5"/>
       <c r="D186" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E186" s="12">
-        <v>7703039366</v>
+        <v>7703039368</v>
       </c>
       <c r="F186" s="21"/>
       <c r="G186" s="21"/>
       <c r="H186" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I186" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J186" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J186" s="5" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>2</v>
-      </c>
-      <c r="B187" s="5" t="s">
+      <c r="B187" s="15"/>
+      <c r="C187" s="15"/>
+      <c r="D187" s="16"/>
+      <c r="E187" s="14"/>
+      <c r="F187" s="22"/>
+      <c r="G187" s="22"/>
+      <c r="H187" s="15"/>
+      <c r="I187" s="16"/>
+      <c r="J187" s="15"/>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>1</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C249" s="5"/>
+      <c r="D249" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E249" s="12">
+        <v>7703039429</v>
+      </c>
+      <c r="F249" s="21"/>
+      <c r="G249" s="21"/>
+      <c r="H249" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C187" s="5"/>
-      <c r="D187" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E187" s="12">
-        <v>7703039367</v>
-      </c>
-      <c r="F187" s="21"/>
-      <c r="G187" s="21"/>
-      <c r="H187" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I187" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J187" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>2</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C188" s="5"/>
-      <c r="D188" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E188" s="12">
-        <v>7703039368</v>
-      </c>
-      <c r="F188" s="21"/>
-      <c r="G188" s="21"/>
-      <c r="H188" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I188" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J188" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B189" s="15"/>
-      <c r="C189" s="15"/>
-      <c r="D189" s="16"/>
-      <c r="E189" s="14"/>
-      <c r="F189" s="22"/>
-      <c r="G189" s="22"/>
-      <c r="H189" s="15"/>
-      <c r="I189" s="16"/>
-      <c r="J189" s="15"/>
+      <c r="I249" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J249" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>1</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C250" s="5"/>
+      <c r="D250" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E250" s="12">
+        <v>7703039430</v>
+      </c>
+      <c r="F250" s="21"/>
+      <c r="G250" s="21"/>
+      <c r="H250" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I250" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J250" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C251" s="5"/>
       <c r="D251" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E251" s="12">
-        <v>7703039429</v>
+        <v>7703039431</v>
       </c>
       <c r="F251" s="21"/>
       <c r="G251" s="21"/>
       <c r="H251" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I251" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J251" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C252" s="5"/>
       <c r="D252" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E252" s="12">
-        <v>7703039430</v>
+        <v>7703039432</v>
       </c>
       <c r="F252" s="21"/>
       <c r="G252" s="21"/>
       <c r="H252" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I252" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J252" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C253" s="5"/>
       <c r="D253" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E253" s="12">
-        <v>7703039431</v>
+        <v>7703039433</v>
       </c>
       <c r="F253" s="21"/>
       <c r="G253" s="21"/>
       <c r="H253" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I253" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J253" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C254" s="5"/>
       <c r="D254" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E254" s="12">
-        <v>7703039432</v>
+        <v>7703039434</v>
       </c>
       <c r="F254" s="21"/>
       <c r="G254" s="21"/>
       <c r="H254" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I254" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J254" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C255" s="5"/>
       <c r="D255" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E255" s="12">
-        <v>7703039433</v>
+        <v>7703039435</v>
       </c>
       <c r="F255" s="21"/>
       <c r="G255" s="21"/>
       <c r="H255" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I255" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J255" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C256" s="5"/>
       <c r="D256" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E256" s="12">
-        <v>7703039434</v>
+        <v>7703039436</v>
       </c>
       <c r="F256" s="21"/>
       <c r="G256" s="21"/>
       <c r="H256" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I256" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J256" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C257" s="5"/>
       <c r="D257" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E257" s="12">
-        <v>7703039435</v>
+        <v>7703039437</v>
       </c>
       <c r="F257" s="21"/>
       <c r="G257" s="21"/>
       <c r="H257" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I257" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J257" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C258" s="5"/>
       <c r="D258" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E258" s="12">
-        <v>7703039436</v>
+        <v>7703039438</v>
       </c>
       <c r="F258" s="21"/>
       <c r="G258" s="21"/>
       <c r="H258" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I258" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J258" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C259" s="5"/>
       <c r="D259" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E259" s="12">
-        <v>7703039437</v>
+        <v>7703039439</v>
       </c>
       <c r="F259" s="21"/>
       <c r="G259" s="21"/>
       <c r="H259" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I259" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J259" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C260" s="5"/>
       <c r="D260" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E260" s="12">
-        <v>7703039438</v>
+        <v>7703039440</v>
       </c>
       <c r="F260" s="21"/>
       <c r="G260" s="21"/>
       <c r="H260" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I260" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J260" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C261" s="5"/>
       <c r="D261" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E261" s="12">
-        <v>7703039439</v>
+        <v>7703039441</v>
       </c>
       <c r="F261" s="21"/>
       <c r="G261" s="21"/>
       <c r="H261" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I261" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J261" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C262" s="5"/>
       <c r="D262" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E262" s="12">
-        <v>7703039440</v>
+        <v>7703039442</v>
       </c>
       <c r="F262" s="21"/>
       <c r="G262" s="21"/>
       <c r="H262" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I262" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J262" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C263" s="5"/>
       <c r="D263" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E263" s="12">
-        <v>7703039441</v>
+        <v>7703039443</v>
       </c>
       <c r="F263" s="21"/>
       <c r="G263" s="21"/>
       <c r="H263" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I263" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J263" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C264" s="5"/>
       <c r="D264" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E264" s="12">
-        <v>7703039442</v>
+        <v>7703039444</v>
       </c>
       <c r="F264" s="21"/>
       <c r="G264" s="21"/>
       <c r="H264" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I264" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J264" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C265" s="5"/>
       <c r="D265" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E265" s="12">
-        <v>7703039443</v>
+        <v>7703039445</v>
       </c>
       <c r="F265" s="21"/>
       <c r="G265" s="21"/>
       <c r="H265" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I265" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J265" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C266" s="5"/>
       <c r="D266" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E266" s="12">
-        <v>7703039444</v>
+        <v>7703039446</v>
       </c>
       <c r="F266" s="21"/>
       <c r="G266" s="21"/>
       <c r="H266" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I266" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J266" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C267" s="5"/>
       <c r="D267" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E267" s="12">
-        <v>7703039445</v>
+        <v>7703039447</v>
       </c>
       <c r="F267" s="21"/>
       <c r="G267" s="21"/>
       <c r="H267" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I267" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J267" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C268" s="5"/>
       <c r="D268" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E268" s="12">
-        <v>7703039446</v>
+        <v>7703039448</v>
       </c>
       <c r="F268" s="21"/>
       <c r="G268" s="21"/>
       <c r="H268" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I268" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J268" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C269" s="5"/>
       <c r="D269" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E269" s="12">
-        <v>7703039447</v>
+        <v>7703039449</v>
       </c>
       <c r="F269" s="21"/>
       <c r="G269" s="21"/>
       <c r="H269" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I269" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J269" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C270" s="5"/>
       <c r="D270" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E270" s="12">
-        <v>7703039448</v>
+        <v>7703039450</v>
       </c>
       <c r="F270" s="21"/>
       <c r="G270" s="21"/>
       <c r="H270" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I270" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J270" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C271" s="5"/>
       <c r="D271" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E271" s="12">
-        <v>7703039449</v>
+        <v>7703039451</v>
       </c>
       <c r="F271" s="21"/>
       <c r="G271" s="21"/>
       <c r="H271" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I271" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J271" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C272" s="5"/>
       <c r="D272" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E272" s="12">
-        <v>7703039450</v>
+        <v>7703039452</v>
       </c>
       <c r="F272" s="21"/>
       <c r="G272" s="21"/>
       <c r="H272" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I272" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J272" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C273" s="5"/>
       <c r="D273" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E273" s="12">
-        <v>7703039451</v>
+        <v>7703039453</v>
       </c>
       <c r="F273" s="21"/>
       <c r="G273" s="21"/>
       <c r="H273" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I273" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J273" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C274" s="5"/>
       <c r="D274" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E274" s="12">
-        <v>7703039452</v>
+        <v>7703039454</v>
       </c>
       <c r="F274" s="21"/>
       <c r="G274" s="21"/>
       <c r="H274" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I274" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J274" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C275" s="5"/>
       <c r="D275" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E275" s="12">
-        <v>7703039453</v>
+        <v>7703039455</v>
       </c>
       <c r="F275" s="21"/>
       <c r="G275" s="21"/>
       <c r="H275" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I275" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J275" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C276" s="5"/>
       <c r="D276" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E276" s="12">
-        <v>7703039454</v>
+        <v>7703039456</v>
       </c>
       <c r="F276" s="21"/>
       <c r="G276" s="21"/>
       <c r="H276" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I276" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J276" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C277" s="5"/>
       <c r="D277" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E277" s="12">
-        <v>7703039455</v>
+        <v>7703039457</v>
       </c>
       <c r="F277" s="21"/>
       <c r="G277" s="21"/>
       <c r="H277" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I277" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J277" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C278" s="5"/>
       <c r="D278" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E278" s="12">
-        <v>7703039456</v>
+        <v>7703039458</v>
       </c>
       <c r="F278" s="21"/>
       <c r="G278" s="21"/>
       <c r="H278" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I278" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J278" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C279" s="5"/>
       <c r="D279" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E279" s="12">
-        <v>7703039457</v>
+        <v>7703039459</v>
       </c>
       <c r="F279" s="21"/>
       <c r="G279" s="21"/>
       <c r="H279" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I279" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J279" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C280" s="5"/>
       <c r="D280" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E280" s="12">
-        <v>7703039458</v>
+        <v>7703039460</v>
       </c>
       <c r="F280" s="21"/>
       <c r="G280" s="21"/>
       <c r="H280" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I280" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J280" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C281" s="5"/>
       <c r="D281" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E281" s="12">
-        <v>7703039459</v>
+        <v>7703039461</v>
       </c>
       <c r="F281" s="21"/>
       <c r="G281" s="21"/>
       <c r="H281" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I281" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J281" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C282" s="5"/>
       <c r="D282" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E282" s="12">
-        <v>7703039460</v>
+        <v>7703039462</v>
       </c>
       <c r="F282" s="21"/>
       <c r="G282" s="21"/>
       <c r="H282" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I282" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J282" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C283" s="5"/>
       <c r="D283" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E283" s="12">
-        <v>7703039461</v>
+        <v>7703039463</v>
       </c>
       <c r="F283" s="21"/>
       <c r="G283" s="21"/>
       <c r="H283" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I283" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J283" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C284" s="5"/>
       <c r="D284" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E284" s="12">
-        <v>7703039462</v>
+        <v>7703039464</v>
       </c>
       <c r="F284" s="21"/>
       <c r="G284" s="21"/>
       <c r="H284" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I284" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J284" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C285" s="5"/>
       <c r="D285" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E285" s="12">
-        <v>7703039463</v>
+        <v>7703039465</v>
       </c>
       <c r="F285" s="21"/>
       <c r="G285" s="21"/>
       <c r="H285" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I285" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J285" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C286" s="5"/>
       <c r="D286" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E286" s="12">
-        <v>7703039464</v>
+        <v>7703039466</v>
       </c>
       <c r="F286" s="21"/>
       <c r="G286" s="21"/>
       <c r="H286" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I286" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J286" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C287" s="5"/>
       <c r="D287" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E287" s="12">
-        <v>7703039465</v>
+        <v>7703039467</v>
       </c>
       <c r="F287" s="21"/>
       <c r="G287" s="21"/>
       <c r="H287" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I287" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J287" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>2</v>
-      </c>
-      <c r="B288" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C288" s="5"/>
-      <c r="D288" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E288" s="12">
-        <v>7703039466</v>
-      </c>
-      <c r="F288" s="21"/>
-      <c r="G288" s="21"/>
-      <c r="H288" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I288" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J288" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>2</v>
-      </c>
-      <c r="B289" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C289" s="5"/>
-      <c r="D289" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E289" s="12">
-        <v>7703039467</v>
-      </c>
-      <c r="F289" s="21"/>
-      <c r="G289" s="21"/>
-      <c r="H289" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B288" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288" s="8"/>
+      <c r="D288" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E288" s="13">
+        <v>7703039468</v>
+      </c>
+      <c r="F288" s="23"/>
+      <c r="G288" s="23"/>
+      <c r="H288" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I289" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J289" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="290" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A290" t="s">
-        <v>2</v>
-      </c>
-      <c r="B290" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C290" s="8"/>
-      <c r="D290" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E290" s="13">
-        <v>7703039468</v>
-      </c>
-      <c r="F290" s="23"/>
-      <c r="G290" s="23"/>
-      <c r="H290" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I290" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J290" s="8" t="s">
-        <v>48</v>
+      <c r="I288" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J288" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Titre De Séjour Visiteur Avec Renouvellement
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E750830-7B86-4B9F-B9F1-12EFA5048120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43B9393-D15D-4B5D-8A18-1B7E5945B6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="615" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
@@ -925,7 +925,7 @@
   <dimension ref="A1:J288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="11">
-        <v>7703039887</v>
+        <v>7703039888</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>61</v>
@@ -2741,6 +2741,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1a0cd919-d361-40f9-9afc-7bc6ff95d333" xsi:nil="true"/>
@@ -2749,15 +2758,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2956,20 +2956,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1A5563-A825-4419-97ED-5452D9012A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1a0cd919-d361-40f9-9afc-7bc6ff95d333"/>
     <ds:schemaRef ds:uri="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Commit New JDD Titre Visiteur Renouvellement
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43B9393-D15D-4B5D-8A18-1B7E5945B6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C6F37-FA1F-4DDF-9ADF-C07822135BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="615" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
@@ -925,7 +925,7 @@
   <dimension ref="A1:J288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="11">
-        <v>7703039888</v>
+        <v>7703039890</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>61</v>
@@ -2741,15 +2741,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1a0cd919-d361-40f9-9afc-7bc6ff95d333" xsi:nil="true"/>
@@ -2758,6 +2749,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2956,20 +2956,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1A5563-A825-4419-97ED-5452D9012A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1a0cd919-d361-40f9-9afc-7bc6ff95d333"/>
     <ds:schemaRef ds:uri="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Commit Correction Dossier Downloads
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254C6F37-FA1F-4DDF-9ADF-C07822135BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE23A76-F85A-4242-9D10-C1C047DBF114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,7 +925,7 @@
   <dimension ref="A1:J288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="11">
-        <v>7703039890</v>
+        <v>7703039891</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>61</v>
@@ -2741,6 +2741,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1a0cd919-d361-40f9-9afc-7bc6ff95d333" xsi:nil="true"/>
@@ -2749,15 +2758,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2956,20 +2956,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1A5563-A825-4419-97ED-5452D9012A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1a0cd919-d361-40f9-9afc-7bc6ff95d333"/>
     <ds:schemaRef ds:uri="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Ajout des vérifs AGDREF
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C91F4-1AE7-4CD7-AB3B-C55F0E54432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE82B6F-FD47-4C38-BBAB-20660DA63C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$288</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$J$287</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="69">
   <si>
     <t>Usager</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>23/12/2023</t>
+  </si>
+  <si>
+    <t>23/12/20223</t>
   </si>
 </sst>
 </file>
@@ -934,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J288"/>
+  <dimension ref="A1:J287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,13 +1003,13 @@
         <v>64</v>
       </c>
       <c r="E2" s="11">
-        <v>7703040652</v>
+        <v>7703040664</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>59</v>
@@ -1029,16 +1032,16 @@
         <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="E3" s="11">
-        <v>7703039879</v>
+        <v>7703040665</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>59</v>
@@ -1055,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>58</v>
@@ -1064,7 +1067,7 @@
         <v>64</v>
       </c>
       <c r="E4" s="11">
-        <v>7703040653</v>
+        <v>7703040666</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>66</v>
@@ -1087,22 +1090,22 @@
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>7703040654</v>
+        <v>7703039883</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>59</v>
@@ -1114,6 +1117,32 @@
         <v>56</v>
       </c>
     </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="5"/>
+      <c r="D160" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E160" s="12">
+        <v>7703039343</v>
+      </c>
+      <c r="F160" s="21"/>
+      <c r="G160" s="21"/>
+      <c r="H160" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I160" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J160" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>1</v>
@@ -1126,12 +1155,12 @@
         <v>1</v>
       </c>
       <c r="E161" s="12">
-        <v>7703039343</v>
+        <v>7703039344</v>
       </c>
       <c r="F161" s="21"/>
       <c r="G161" s="21"/>
       <c r="H161" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I161" s="6" t="s">
         <v>44</v>
@@ -1152,12 +1181,12 @@
         <v>1</v>
       </c>
       <c r="E162" s="12">
-        <v>7703039344</v>
+        <v>7703039345</v>
       </c>
       <c r="F162" s="21"/>
       <c r="G162" s="21"/>
       <c r="H162" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I162" s="6" t="s">
         <v>44</v>
@@ -1178,12 +1207,12 @@
         <v>1</v>
       </c>
       <c r="E163" s="12">
-        <v>7703039345</v>
+        <v>7703039346</v>
       </c>
       <c r="F163" s="21"/>
       <c r="G163" s="21"/>
       <c r="H163" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I163" s="6" t="s">
         <v>44</v>
@@ -1204,12 +1233,12 @@
         <v>1</v>
       </c>
       <c r="E164" s="12">
-        <v>7703039346</v>
+        <v>7703039347</v>
       </c>
       <c r="F164" s="21"/>
       <c r="G164" s="21"/>
       <c r="H164" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I164" s="6" t="s">
         <v>44</v>
@@ -1230,12 +1259,12 @@
         <v>1</v>
       </c>
       <c r="E165" s="12">
-        <v>7703039347</v>
+        <v>7703039348</v>
       </c>
       <c r="F165" s="21"/>
       <c r="G165" s="21"/>
       <c r="H165" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I165" s="6" t="s">
         <v>44</v>
@@ -1256,12 +1285,12 @@
         <v>1</v>
       </c>
       <c r="E166" s="12">
-        <v>7703039348</v>
+        <v>7703039349</v>
       </c>
       <c r="F166" s="21"/>
       <c r="G166" s="21"/>
       <c r="H166" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I166" s="6" t="s">
         <v>44</v>
@@ -1282,12 +1311,12 @@
         <v>1</v>
       </c>
       <c r="E167" s="12">
-        <v>7703039349</v>
+        <v>7703039350</v>
       </c>
       <c r="F167" s="21"/>
       <c r="G167" s="21"/>
       <c r="H167" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I167" s="6" t="s">
         <v>44</v>
@@ -1308,12 +1337,12 @@
         <v>1</v>
       </c>
       <c r="E168" s="12">
-        <v>7703039350</v>
+        <v>7703039351</v>
       </c>
       <c r="F168" s="21"/>
       <c r="G168" s="21"/>
       <c r="H168" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I168" s="6" t="s">
         <v>44</v>
@@ -1334,12 +1363,12 @@
         <v>1</v>
       </c>
       <c r="E169" s="12">
-        <v>7703039351</v>
+        <v>7703039352</v>
       </c>
       <c r="F169" s="21"/>
       <c r="G169" s="21"/>
       <c r="H169" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I169" s="6" t="s">
         <v>44</v>
@@ -1360,12 +1389,12 @@
         <v>1</v>
       </c>
       <c r="E170" s="12">
-        <v>7703039352</v>
+        <v>7703039353</v>
       </c>
       <c r="F170" s="21"/>
       <c r="G170" s="21"/>
       <c r="H170" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I170" s="6" t="s">
         <v>44</v>
@@ -1386,12 +1415,12 @@
         <v>1</v>
       </c>
       <c r="E171" s="12">
-        <v>7703039353</v>
+        <v>7703039354</v>
       </c>
       <c r="F171" s="21"/>
       <c r="G171" s="21"/>
       <c r="H171" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I171" s="6" t="s">
         <v>44</v>
@@ -1412,12 +1441,12 @@
         <v>1</v>
       </c>
       <c r="E172" s="12">
-        <v>7703039354</v>
+        <v>7703039355</v>
       </c>
       <c r="F172" s="21"/>
       <c r="G172" s="21"/>
       <c r="H172" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I172" s="6" t="s">
         <v>44</v>
@@ -1438,12 +1467,12 @@
         <v>1</v>
       </c>
       <c r="E173" s="12">
-        <v>7703039355</v>
+        <v>7703039356</v>
       </c>
       <c r="F173" s="21"/>
       <c r="G173" s="21"/>
       <c r="H173" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I173" s="6" t="s">
         <v>44</v>
@@ -1464,12 +1493,12 @@
         <v>1</v>
       </c>
       <c r="E174" s="12">
-        <v>7703039356</v>
+        <v>7703039357</v>
       </c>
       <c r="F174" s="21"/>
       <c r="G174" s="21"/>
       <c r="H174" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I174" s="6" t="s">
         <v>44</v>
@@ -1490,12 +1519,12 @@
         <v>1</v>
       </c>
       <c r="E175" s="12">
-        <v>7703039357</v>
+        <v>7703039358</v>
       </c>
       <c r="F175" s="21"/>
       <c r="G175" s="21"/>
       <c r="H175" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I175" s="6" t="s">
         <v>44</v>
@@ -1516,12 +1545,12 @@
         <v>1</v>
       </c>
       <c r="E176" s="12">
-        <v>7703039358</v>
+        <v>7703039359</v>
       </c>
       <c r="F176" s="21"/>
       <c r="G176" s="21"/>
       <c r="H176" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I176" s="6" t="s">
         <v>44</v>
@@ -1542,12 +1571,12 @@
         <v>1</v>
       </c>
       <c r="E177" s="12">
-        <v>7703039359</v>
+        <v>7703039360</v>
       </c>
       <c r="F177" s="21"/>
       <c r="G177" s="21"/>
       <c r="H177" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I177" s="6" t="s">
         <v>44</v>
@@ -1568,12 +1597,12 @@
         <v>1</v>
       </c>
       <c r="E178" s="12">
-        <v>7703039360</v>
+        <v>7703039361</v>
       </c>
       <c r="F178" s="21"/>
       <c r="G178" s="21"/>
       <c r="H178" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I178" s="6" t="s">
         <v>44</v>
@@ -1594,12 +1623,12 @@
         <v>1</v>
       </c>
       <c r="E179" s="12">
-        <v>7703039361</v>
+        <v>7703039362</v>
       </c>
       <c r="F179" s="21"/>
       <c r="G179" s="21"/>
       <c r="H179" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I179" s="6" t="s">
         <v>44</v>
@@ -1620,12 +1649,12 @@
         <v>1</v>
       </c>
       <c r="E180" s="12">
-        <v>7703039362</v>
+        <v>7703039363</v>
       </c>
       <c r="F180" s="21"/>
       <c r="G180" s="21"/>
       <c r="H180" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I180" s="6" t="s">
         <v>44</v>
@@ -1646,12 +1675,12 @@
         <v>1</v>
       </c>
       <c r="E181" s="12">
-        <v>7703039363</v>
+        <v>7703039364</v>
       </c>
       <c r="F181" s="21"/>
       <c r="G181" s="21"/>
       <c r="H181" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I181" s="6" t="s">
         <v>44</v>
@@ -1672,12 +1701,12 @@
         <v>1</v>
       </c>
       <c r="E182" s="12">
-        <v>7703039364</v>
+        <v>7703039365</v>
       </c>
       <c r="F182" s="21"/>
       <c r="G182" s="21"/>
       <c r="H182" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I182" s="6" t="s">
         <v>44</v>
@@ -1698,12 +1727,12 @@
         <v>1</v>
       </c>
       <c r="E183" s="12">
-        <v>7703039365</v>
+        <v>7703039366</v>
       </c>
       <c r="F183" s="21"/>
       <c r="G183" s="21"/>
       <c r="H183" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I183" s="6" t="s">
         <v>44</v>
@@ -1724,12 +1753,12 @@
         <v>1</v>
       </c>
       <c r="E184" s="12">
-        <v>7703039366</v>
+        <v>7703039367</v>
       </c>
       <c r="F184" s="21"/>
       <c r="G184" s="21"/>
       <c r="H184" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I184" s="6" t="s">
         <v>44</v>
@@ -1750,12 +1779,12 @@
         <v>1</v>
       </c>
       <c r="E185" s="12">
-        <v>7703039367</v>
+        <v>7703039368</v>
       </c>
       <c r="F185" s="21"/>
       <c r="G185" s="21"/>
       <c r="H185" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I185" s="6" t="s">
         <v>44</v>
@@ -1765,41 +1794,41 @@
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>1</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C186" s="5"/>
-      <c r="D186" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E186" s="12">
-        <v>7703039368</v>
-      </c>
-      <c r="F186" s="21"/>
-      <c r="G186" s="21"/>
-      <c r="H186" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I186" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J186" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B187" s="15"/>
-      <c r="C187" s="15"/>
-      <c r="D187" s="16"/>
-      <c r="E187" s="14"/>
-      <c r="F187" s="22"/>
-      <c r="G187" s="22"/>
-      <c r="H187" s="15"/>
-      <c r="I187" s="16"/>
-      <c r="J187" s="15"/>
+      <c r="B186" s="15"/>
+      <c r="C186" s="15"/>
+      <c r="D186" s="16"/>
+      <c r="E186" s="14"/>
+      <c r="F186" s="22"/>
+      <c r="G186" s="22"/>
+      <c r="H186" s="15"/>
+      <c r="I186" s="16"/>
+      <c r="J186" s="15"/>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>1</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C248" s="5"/>
+      <c r="D248" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E248" s="12">
+        <v>7703039429</v>
+      </c>
+      <c r="F248" s="21"/>
+      <c r="G248" s="21"/>
+      <c r="H248" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I248" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J248" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
@@ -1813,12 +1842,12 @@
         <v>1</v>
       </c>
       <c r="E249" s="12">
-        <v>7703039429</v>
+        <v>7703039430</v>
       </c>
       <c r="F249" s="21"/>
       <c r="G249" s="21"/>
       <c r="H249" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I249" s="6" t="s">
         <v>46</v>
@@ -1839,12 +1868,12 @@
         <v>1</v>
       </c>
       <c r="E250" s="12">
-        <v>7703039430</v>
+        <v>7703039431</v>
       </c>
       <c r="F250" s="21"/>
       <c r="G250" s="21"/>
       <c r="H250" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I250" s="6" t="s">
         <v>46</v>
@@ -1865,12 +1894,12 @@
         <v>1</v>
       </c>
       <c r="E251" s="12">
-        <v>7703039431</v>
+        <v>7703039432</v>
       </c>
       <c r="F251" s="21"/>
       <c r="G251" s="21"/>
       <c r="H251" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I251" s="6" t="s">
         <v>46</v>
@@ -1891,12 +1920,12 @@
         <v>1</v>
       </c>
       <c r="E252" s="12">
-        <v>7703039432</v>
+        <v>7703039433</v>
       </c>
       <c r="F252" s="21"/>
       <c r="G252" s="21"/>
       <c r="H252" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I252" s="6" t="s">
         <v>46</v>
@@ -1917,12 +1946,12 @@
         <v>1</v>
       </c>
       <c r="E253" s="12">
-        <v>7703039433</v>
+        <v>7703039434</v>
       </c>
       <c r="F253" s="21"/>
       <c r="G253" s="21"/>
       <c r="H253" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I253" s="6" t="s">
         <v>46</v>
@@ -1943,12 +1972,12 @@
         <v>1</v>
       </c>
       <c r="E254" s="12">
-        <v>7703039434</v>
+        <v>7703039435</v>
       </c>
       <c r="F254" s="21"/>
       <c r="G254" s="21"/>
       <c r="H254" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I254" s="6" t="s">
         <v>46</v>
@@ -1969,12 +1998,12 @@
         <v>1</v>
       </c>
       <c r="E255" s="12">
-        <v>7703039435</v>
+        <v>7703039436</v>
       </c>
       <c r="F255" s="21"/>
       <c r="G255" s="21"/>
       <c r="H255" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I255" s="6" t="s">
         <v>46</v>
@@ -1995,12 +2024,12 @@
         <v>1</v>
       </c>
       <c r="E256" s="12">
-        <v>7703039436</v>
+        <v>7703039437</v>
       </c>
       <c r="F256" s="21"/>
       <c r="G256" s="21"/>
       <c r="H256" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I256" s="6" t="s">
         <v>46</v>
@@ -2021,12 +2050,12 @@
         <v>1</v>
       </c>
       <c r="E257" s="12">
-        <v>7703039437</v>
+        <v>7703039438</v>
       </c>
       <c r="F257" s="21"/>
       <c r="G257" s="21"/>
       <c r="H257" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I257" s="6" t="s">
         <v>46</v>
@@ -2047,12 +2076,12 @@
         <v>1</v>
       </c>
       <c r="E258" s="12">
-        <v>7703039438</v>
+        <v>7703039439</v>
       </c>
       <c r="F258" s="21"/>
       <c r="G258" s="21"/>
       <c r="H258" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I258" s="6" t="s">
         <v>46</v>
@@ -2073,12 +2102,12 @@
         <v>1</v>
       </c>
       <c r="E259" s="12">
-        <v>7703039439</v>
+        <v>7703039440</v>
       </c>
       <c r="F259" s="21"/>
       <c r="G259" s="21"/>
       <c r="H259" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I259" s="6" t="s">
         <v>46</v>
@@ -2099,12 +2128,12 @@
         <v>1</v>
       </c>
       <c r="E260" s="12">
-        <v>7703039440</v>
+        <v>7703039441</v>
       </c>
       <c r="F260" s="21"/>
       <c r="G260" s="21"/>
       <c r="H260" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I260" s="6" t="s">
         <v>46</v>
@@ -2125,12 +2154,12 @@
         <v>1</v>
       </c>
       <c r="E261" s="12">
-        <v>7703039441</v>
+        <v>7703039442</v>
       </c>
       <c r="F261" s="21"/>
       <c r="G261" s="21"/>
       <c r="H261" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I261" s="6" t="s">
         <v>46</v>
@@ -2151,12 +2180,12 @@
         <v>1</v>
       </c>
       <c r="E262" s="12">
-        <v>7703039442</v>
+        <v>7703039443</v>
       </c>
       <c r="F262" s="21"/>
       <c r="G262" s="21"/>
       <c r="H262" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I262" s="6" t="s">
         <v>46</v>
@@ -2177,12 +2206,12 @@
         <v>1</v>
       </c>
       <c r="E263" s="12">
-        <v>7703039443</v>
+        <v>7703039444</v>
       </c>
       <c r="F263" s="21"/>
       <c r="G263" s="21"/>
       <c r="H263" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I263" s="6" t="s">
         <v>46</v>
@@ -2203,12 +2232,12 @@
         <v>1</v>
       </c>
       <c r="E264" s="12">
-        <v>7703039444</v>
+        <v>7703039445</v>
       </c>
       <c r="F264" s="21"/>
       <c r="G264" s="21"/>
       <c r="H264" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I264" s="6" t="s">
         <v>46</v>
@@ -2229,12 +2258,12 @@
         <v>1</v>
       </c>
       <c r="E265" s="12">
-        <v>7703039445</v>
+        <v>7703039446</v>
       </c>
       <c r="F265" s="21"/>
       <c r="G265" s="21"/>
       <c r="H265" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I265" s="6" t="s">
         <v>46</v>
@@ -2255,12 +2284,12 @@
         <v>1</v>
       </c>
       <c r="E266" s="12">
-        <v>7703039446</v>
+        <v>7703039447</v>
       </c>
       <c r="F266" s="21"/>
       <c r="G266" s="21"/>
       <c r="H266" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I266" s="6" t="s">
         <v>46</v>
@@ -2281,12 +2310,12 @@
         <v>1</v>
       </c>
       <c r="E267" s="12">
-        <v>7703039447</v>
+        <v>7703039448</v>
       </c>
       <c r="F267" s="21"/>
       <c r="G267" s="21"/>
       <c r="H267" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I267" s="6" t="s">
         <v>46</v>
@@ -2307,12 +2336,12 @@
         <v>1</v>
       </c>
       <c r="E268" s="12">
-        <v>7703039448</v>
+        <v>7703039449</v>
       </c>
       <c r="F268" s="21"/>
       <c r="G268" s="21"/>
       <c r="H268" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I268" s="6" t="s">
         <v>46</v>
@@ -2333,12 +2362,12 @@
         <v>1</v>
       </c>
       <c r="E269" s="12">
-        <v>7703039449</v>
+        <v>7703039450</v>
       </c>
       <c r="F269" s="21"/>
       <c r="G269" s="21"/>
       <c r="H269" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I269" s="6" t="s">
         <v>46</v>
@@ -2359,12 +2388,12 @@
         <v>1</v>
       </c>
       <c r="E270" s="12">
-        <v>7703039450</v>
+        <v>7703039451</v>
       </c>
       <c r="F270" s="21"/>
       <c r="G270" s="21"/>
       <c r="H270" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I270" s="6" t="s">
         <v>46</v>
@@ -2385,12 +2414,12 @@
         <v>1</v>
       </c>
       <c r="E271" s="12">
-        <v>7703039451</v>
+        <v>7703039452</v>
       </c>
       <c r="F271" s="21"/>
       <c r="G271" s="21"/>
       <c r="H271" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I271" s="6" t="s">
         <v>46</v>
@@ -2411,12 +2440,12 @@
         <v>1</v>
       </c>
       <c r="E272" s="12">
-        <v>7703039452</v>
+        <v>7703039453</v>
       </c>
       <c r="F272" s="21"/>
       <c r="G272" s="21"/>
       <c r="H272" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I272" s="6" t="s">
         <v>46</v>
@@ -2437,12 +2466,12 @@
         <v>1</v>
       </c>
       <c r="E273" s="12">
-        <v>7703039453</v>
+        <v>7703039454</v>
       </c>
       <c r="F273" s="21"/>
       <c r="G273" s="21"/>
       <c r="H273" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I273" s="6" t="s">
         <v>46</v>
@@ -2463,12 +2492,12 @@
         <v>1</v>
       </c>
       <c r="E274" s="12">
-        <v>7703039454</v>
+        <v>7703039455</v>
       </c>
       <c r="F274" s="21"/>
       <c r="G274" s="21"/>
       <c r="H274" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I274" s="6" t="s">
         <v>46</v>
@@ -2489,12 +2518,12 @@
         <v>1</v>
       </c>
       <c r="E275" s="12">
-        <v>7703039455</v>
+        <v>7703039456</v>
       </c>
       <c r="F275" s="21"/>
       <c r="G275" s="21"/>
       <c r="H275" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I275" s="6" t="s">
         <v>46</v>
@@ -2515,12 +2544,12 @@
         <v>1</v>
       </c>
       <c r="E276" s="12">
-        <v>7703039456</v>
+        <v>7703039457</v>
       </c>
       <c r="F276" s="21"/>
       <c r="G276" s="21"/>
       <c r="H276" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I276" s="6" t="s">
         <v>46</v>
@@ -2541,12 +2570,12 @@
         <v>1</v>
       </c>
       <c r="E277" s="12">
-        <v>7703039457</v>
+        <v>7703039458</v>
       </c>
       <c r="F277" s="21"/>
       <c r="G277" s="21"/>
       <c r="H277" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I277" s="6" t="s">
         <v>46</v>
@@ -2567,12 +2596,12 @@
         <v>1</v>
       </c>
       <c r="E278" s="12">
-        <v>7703039458</v>
+        <v>7703039459</v>
       </c>
       <c r="F278" s="21"/>
       <c r="G278" s="21"/>
       <c r="H278" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I278" s="6" t="s">
         <v>46</v>
@@ -2593,12 +2622,12 @@
         <v>1</v>
       </c>
       <c r="E279" s="12">
-        <v>7703039459</v>
+        <v>7703039460</v>
       </c>
       <c r="F279" s="21"/>
       <c r="G279" s="21"/>
       <c r="H279" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I279" s="6" t="s">
         <v>46</v>
@@ -2619,12 +2648,12 @@
         <v>1</v>
       </c>
       <c r="E280" s="12">
-        <v>7703039460</v>
+        <v>7703039461</v>
       </c>
       <c r="F280" s="21"/>
       <c r="G280" s="21"/>
       <c r="H280" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I280" s="6" t="s">
         <v>46</v>
@@ -2645,12 +2674,12 @@
         <v>1</v>
       </c>
       <c r="E281" s="12">
-        <v>7703039461</v>
+        <v>7703039462</v>
       </c>
       <c r="F281" s="21"/>
       <c r="G281" s="21"/>
       <c r="H281" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I281" s="6" t="s">
         <v>46</v>
@@ -2671,12 +2700,12 @@
         <v>1</v>
       </c>
       <c r="E282" s="12">
-        <v>7703039462</v>
+        <v>7703039463</v>
       </c>
       <c r="F282" s="21"/>
       <c r="G282" s="21"/>
       <c r="H282" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I282" s="6" t="s">
         <v>46</v>
@@ -2697,12 +2726,12 @@
         <v>1</v>
       </c>
       <c r="E283" s="12">
-        <v>7703039463</v>
+        <v>7703039464</v>
       </c>
       <c r="F283" s="21"/>
       <c r="G283" s="21"/>
       <c r="H283" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I283" s="6" t="s">
         <v>46</v>
@@ -2723,12 +2752,12 @@
         <v>1</v>
       </c>
       <c r="E284" s="12">
-        <v>7703039464</v>
+        <v>7703039465</v>
       </c>
       <c r="F284" s="21"/>
       <c r="G284" s="21"/>
       <c r="H284" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I284" s="6" t="s">
         <v>46</v>
@@ -2749,12 +2778,12 @@
         <v>1</v>
       </c>
       <c r="E285" s="12">
-        <v>7703039465</v>
+        <v>7703039466</v>
       </c>
       <c r="F285" s="21"/>
       <c r="G285" s="21"/>
       <c r="H285" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I285" s="6" t="s">
         <v>46</v>
@@ -2775,12 +2804,12 @@
         <v>1</v>
       </c>
       <c r="E286" s="12">
-        <v>7703039466</v>
+        <v>7703039467</v>
       </c>
       <c r="F286" s="21"/>
       <c r="G286" s="21"/>
       <c r="H286" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I286" s="6" t="s">
         <v>46</v>
@@ -2789,55 +2818,29 @@
         <v>47</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>1</v>
       </c>
-      <c r="B287" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C287" s="5"/>
-      <c r="D287" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E287" s="12">
-        <v>7703039467</v>
-      </c>
-      <c r="F287" s="21"/>
-      <c r="G287" s="21"/>
-      <c r="H287" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I287" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J287" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" t="s">
-        <v>1</v>
-      </c>
-      <c r="B288" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C288" s="8"/>
-      <c r="D288" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E288" s="13">
+      <c r="B287" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C287" s="8"/>
+      <c r="D287" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E287" s="13">
         <v>7703039468</v>
       </c>
-      <c r="F288" s="23"/>
-      <c r="G288" s="23"/>
-      <c r="H288" s="8" t="s">
+      <c r="F287" s="23"/>
+      <c r="G287" s="23"/>
+      <c r="H287" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I288" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J288" s="8" t="s">
+      <c r="I287" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J287" s="8" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gérer les données de la création d'un compte
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE82B6F-FD47-4C38-BBAB-20660DA63C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E13AC6-53E6-4E46-8EF5-37F275002176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="68">
   <si>
     <t>Usager</t>
   </si>
@@ -227,9 +227,6 @@
     <t>01/12/2022</t>
   </si>
   <si>
-    <t>30/11/2023</t>
-  </si>
-  <si>
     <t>RenouvellementDeTitreSejour</t>
   </si>
   <si>
@@ -245,7 +242,7 @@
     <t>23/12/2023</t>
   </si>
   <si>
-    <t>23/12/20223</t>
+    <t>30/11/2022</t>
   </si>
 </sst>
 </file>
@@ -940,7 +937,7 @@
   <dimension ref="A1:J287"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,22 +991,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="11">
-        <v>7703040664</v>
+        <v>7703040673</v>
       </c>
       <c r="F2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>68</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>59</v>
@@ -1026,22 +1023,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="11">
-        <v>7703040665</v>
+        <v>7703040671</v>
       </c>
       <c r="F3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>59</v>
@@ -1064,16 +1061,16 @@
         <v>58</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="11">
-        <v>7703040666</v>
+        <v>7703040674</v>
       </c>
       <c r="F4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>59</v>
@@ -1090,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>58</v>
@@ -1099,13 +1096,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>7703039883</v>
+        <v>7703039885</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>61</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>59</v>
@@ -2852,6 +2849,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1a0cd919-d361-40f9-9afc-7bc6ff95d333" xsi:nil="true"/>
@@ -2860,15 +2866,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3067,20 +3064,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1A5563-A825-4419-97ED-5452D9012A3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1a0cd919-d361-40f9-9afc-7bc6ff95d333"/>
     <ds:schemaRef ds:uri="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Test Issam Preprod 29/11/2023
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhizaoui\.git\NewProject29092023\Nouveau dossier1\22_11\ANEF-AutomatizationProject\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISSAM.RHARBAOUI\git\WORKSPACE\ANEF-AutomatizationProject\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2228ED-3F5B-402D-9D22-522EEB1E2D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309F7331-7CEA-4A96-9686-3643E6A19083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72" yWindow="2748" windowWidth="21072" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JDD" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$K$277</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JDD!$A$1:$K$278</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="82">
   <si>
     <t>Usager</t>
   </si>
@@ -227,12 +227,6 @@
     <t>Etudiant</t>
   </si>
   <si>
-    <t>24/12/2022</t>
-  </si>
-  <si>
-    <t>23/12/2023</t>
-  </si>
-  <si>
     <t>EnvExec</t>
   </si>
   <si>
@@ -284,13 +278,13 @@
     <t>RenouvellementDeTitreSejour</t>
   </si>
   <si>
-    <t>01/12/2022</t>
-  </si>
-  <si>
-    <t>30/11/2022</t>
-  </si>
-  <si>
-    <t>URL_ANEFQualif</t>
+    <t>URL_ANEFPreProd</t>
+  </si>
+  <si>
+    <t>15/01/2023</t>
+  </si>
+  <si>
+    <t>14/01/2024</t>
   </si>
 </sst>
 </file>
@@ -837,9 +831,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -877,9 +871,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -912,26 +906,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -964,26 +941,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1157,32 +1117,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L277"/>
+  <dimension ref="A1:L278"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="3" width="75.5703125" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="45.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="75.5546875" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="45.33203125" customWidth="1"/>
     <col min="10" max="10" width="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>53</v>
@@ -1212,15 +1172,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>58</v>
@@ -1229,13 +1189,13 @@
         <v>61</v>
       </c>
       <c r="F2" s="8">
-        <v>7703040985</v>
+        <v>7703042981</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>59</v>
@@ -1244,19 +1204,19 @@
         <v>54</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>58</v>
@@ -1265,34 +1225,34 @@
         <v>61</v>
       </c>
       <c r="F3" s="8">
-        <v>7703040986</v>
+        <v>7703042982</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K3" s="35" t="s">
         <v>56</v>
       </c>
       <c r="L3" s="36"/>
     </row>
-    <row r="4" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>58</v>
@@ -1301,31 +1261,31 @@
         <v>61</v>
       </c>
       <c r="F4" s="8">
-        <v>7703040987</v>
+        <v>7703042983</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K4" s="35" t="s">
         <v>56</v>
       </c>
       <c r="L4" s="36"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
@@ -1334,16 +1294,16 @@
         <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="F5" s="8">
-        <v>7703040988</v>
+        <v>7703042275</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>59</v>
@@ -1355,156 +1315,156 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="8">
-        <v>7703040989</v>
-      </c>
-      <c r="G6" s="40" t="s">
+        <v>7703042985</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+    </row>
+    <row r="7" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="8">
-        <v>7703040990</v>
+        <v>7703042986</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="D8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="8">
+        <v>7703042987</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="32" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+    <row r="9" spans="1:12" s="32" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E9" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="8">
-        <v>7703040991</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="28" t="s">
+      <c r="F9" s="8">
+        <v>7703042988</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J9" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K9" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="8">
-        <v>7703040992</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>58</v>
@@ -1513,13 +1473,13 @@
         <v>61</v>
       </c>
       <c r="F10" s="8">
-        <v>7703040993</v>
+        <v>7703042989</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>59</v>
@@ -1531,15 +1491,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>58</v>
@@ -1548,15 +1508,15 @@
         <v>61</v>
       </c>
       <c r="F11" s="8">
-        <v>7703040994</v>
+        <v>7703042990</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J11" s="14" t="s">
@@ -1566,51 +1526,50 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F12" s="8">
-        <v>7703040995</v>
+        <v>7703042991</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="36"/>
-    </row>
-    <row r="13" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>58</v>
@@ -1619,34 +1578,34 @@
         <v>61</v>
       </c>
       <c r="F13" s="8">
-        <v>7703040996</v>
+        <v>7703042992</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="K13" s="35" t="s">
         <v>56</v>
       </c>
       <c r="L13" s="36"/>
     </row>
-    <row r="14" spans="1:12" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>58</v>
@@ -1655,90 +1614,97 @@
         <v>61</v>
       </c>
       <c r="F14" s="8">
-        <v>7703040997</v>
+        <v>7703042993</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K14" s="35" t="s">
         <v>56</v>
       </c>
       <c r="L14" s="36"/>
     </row>
-    <row r="15" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:12" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="8">
-        <v>7703040998</v>
+        <v>7703042994</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="36"/>
+    </row>
+    <row r="16" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="8">
+        <v>7703042995</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="K16" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>1</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D150" s="3"/>
-      <c r="E150" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F150" s="9">
-        <v>7703039343</v>
-      </c>
-      <c r="G150" s="17"/>
-      <c r="H150" s="17"/>
-      <c r="I150" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J150" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K150" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -1753,12 +1719,12 @@
         <v>1</v>
       </c>
       <c r="F151" s="9">
-        <v>7703039344</v>
+        <v>7703039343</v>
       </c>
       <c r="G151" s="17"/>
       <c r="H151" s="17"/>
       <c r="I151" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J151" s="4" t="s">
         <v>44</v>
@@ -1767,7 +1733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>1</v>
       </c>
@@ -1782,12 +1748,12 @@
         <v>1</v>
       </c>
       <c r="F152" s="9">
-        <v>7703039345</v>
+        <v>7703039344</v>
       </c>
       <c r="G152" s="17"/>
       <c r="H152" s="17"/>
       <c r="I152" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J152" s="4" t="s">
         <v>44</v>
@@ -1796,7 +1762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -1811,12 +1777,12 @@
         <v>1</v>
       </c>
       <c r="F153" s="9">
-        <v>7703039346</v>
+        <v>7703039345</v>
       </c>
       <c r="G153" s="17"/>
       <c r="H153" s="17"/>
       <c r="I153" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J153" s="4" t="s">
         <v>44</v>
@@ -1825,7 +1791,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -1840,12 +1806,12 @@
         <v>1</v>
       </c>
       <c r="F154" s="9">
-        <v>7703039347</v>
+        <v>7703039346</v>
       </c>
       <c r="G154" s="17"/>
       <c r="H154" s="17"/>
       <c r="I154" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J154" s="4" t="s">
         <v>44</v>
@@ -1854,7 +1820,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -1869,12 +1835,12 @@
         <v>1</v>
       </c>
       <c r="F155" s="9">
-        <v>7703039348</v>
+        <v>7703039347</v>
       </c>
       <c r="G155" s="17"/>
       <c r="H155" s="17"/>
       <c r="I155" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J155" s="4" t="s">
         <v>44</v>
@@ -1883,7 +1849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -1898,12 +1864,12 @@
         <v>1</v>
       </c>
       <c r="F156" s="9">
-        <v>7703039349</v>
+        <v>7703039348</v>
       </c>
       <c r="G156" s="17"/>
       <c r="H156" s="17"/>
       <c r="I156" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J156" s="4" t="s">
         <v>44</v>
@@ -1912,7 +1878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -1927,12 +1893,12 @@
         <v>1</v>
       </c>
       <c r="F157" s="9">
-        <v>7703039350</v>
+        <v>7703039349</v>
       </c>
       <c r="G157" s="17"/>
       <c r="H157" s="17"/>
       <c r="I157" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J157" s="4" t="s">
         <v>44</v>
@@ -1941,7 +1907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>1</v>
       </c>
@@ -1956,12 +1922,12 @@
         <v>1</v>
       </c>
       <c r="F158" s="9">
-        <v>7703039351</v>
+        <v>7703039350</v>
       </c>
       <c r="G158" s="17"/>
       <c r="H158" s="17"/>
       <c r="I158" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J158" s="4" t="s">
         <v>44</v>
@@ -1970,7 +1936,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>1</v>
       </c>
@@ -1985,12 +1951,12 @@
         <v>1</v>
       </c>
       <c r="F159" s="9">
-        <v>7703039352</v>
+        <v>7703039351</v>
       </c>
       <c r="G159" s="17"/>
       <c r="H159" s="17"/>
       <c r="I159" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J159" s="4" t="s">
         <v>44</v>
@@ -1999,7 +1965,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>1</v>
       </c>
@@ -2014,12 +1980,12 @@
         <v>1</v>
       </c>
       <c r="F160" s="9">
-        <v>7703039353</v>
+        <v>7703039352</v>
       </c>
       <c r="G160" s="17"/>
       <c r="H160" s="17"/>
       <c r="I160" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J160" s="4" t="s">
         <v>44</v>
@@ -2028,7 +1994,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>1</v>
       </c>
@@ -2043,12 +2009,12 @@
         <v>1</v>
       </c>
       <c r="F161" s="9">
-        <v>7703039354</v>
+        <v>7703039353</v>
       </c>
       <c r="G161" s="17"/>
       <c r="H161" s="17"/>
       <c r="I161" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J161" s="4" t="s">
         <v>44</v>
@@ -2057,7 +2023,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>1</v>
       </c>
@@ -2072,12 +2038,12 @@
         <v>1</v>
       </c>
       <c r="F162" s="9">
-        <v>7703039355</v>
+        <v>7703039354</v>
       </c>
       <c r="G162" s="17"/>
       <c r="H162" s="17"/>
       <c r="I162" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J162" s="4" t="s">
         <v>44</v>
@@ -2086,7 +2052,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>1</v>
       </c>
@@ -2101,12 +2067,12 @@
         <v>1</v>
       </c>
       <c r="F163" s="9">
-        <v>7703039356</v>
+        <v>7703039355</v>
       </c>
       <c r="G163" s="17"/>
       <c r="H163" s="17"/>
       <c r="I163" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J163" s="4" t="s">
         <v>44</v>
@@ -2115,7 +2081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>1</v>
       </c>
@@ -2130,12 +2096,12 @@
         <v>1</v>
       </c>
       <c r="F164" s="9">
-        <v>7703039357</v>
+        <v>7703039356</v>
       </c>
       <c r="G164" s="17"/>
       <c r="H164" s="17"/>
       <c r="I164" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J164" s="4" t="s">
         <v>44</v>
@@ -2144,7 +2110,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>1</v>
       </c>
@@ -2159,12 +2125,12 @@
         <v>1</v>
       </c>
       <c r="F165" s="9">
-        <v>7703039358</v>
+        <v>7703039357</v>
       </c>
       <c r="G165" s="17"/>
       <c r="H165" s="17"/>
       <c r="I165" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J165" s="4" t="s">
         <v>44</v>
@@ -2173,7 +2139,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>1</v>
       </c>
@@ -2188,12 +2154,12 @@
         <v>1</v>
       </c>
       <c r="F166" s="9">
-        <v>7703039359</v>
+        <v>7703039358</v>
       </c>
       <c r="G166" s="17"/>
       <c r="H166" s="17"/>
       <c r="I166" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J166" s="4" t="s">
         <v>44</v>
@@ -2202,7 +2168,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>1</v>
       </c>
@@ -2217,12 +2183,12 @@
         <v>1</v>
       </c>
       <c r="F167" s="9">
-        <v>7703039360</v>
+        <v>7703039359</v>
       </c>
       <c r="G167" s="17"/>
       <c r="H167" s="17"/>
       <c r="I167" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J167" s="4" t="s">
         <v>44</v>
@@ -2231,7 +2197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>1</v>
       </c>
@@ -2246,12 +2212,12 @@
         <v>1</v>
       </c>
       <c r="F168" s="9">
-        <v>7703039361</v>
+        <v>7703039360</v>
       </c>
       <c r="G168" s="17"/>
       <c r="H168" s="17"/>
       <c r="I168" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J168" s="4" t="s">
         <v>44</v>
@@ -2260,7 +2226,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>1</v>
       </c>
@@ -2275,12 +2241,12 @@
         <v>1</v>
       </c>
       <c r="F169" s="9">
-        <v>7703039362</v>
+        <v>7703039361</v>
       </c>
       <c r="G169" s="17"/>
       <c r="H169" s="17"/>
       <c r="I169" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J169" s="4" t="s">
         <v>44</v>
@@ -2289,7 +2255,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>1</v>
       </c>
@@ -2304,12 +2270,12 @@
         <v>1</v>
       </c>
       <c r="F170" s="9">
-        <v>7703039363</v>
+        <v>7703039362</v>
       </c>
       <c r="G170" s="17"/>
       <c r="H170" s="17"/>
       <c r="I170" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J170" s="4" t="s">
         <v>44</v>
@@ -2318,7 +2284,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>1</v>
       </c>
@@ -2333,12 +2299,12 @@
         <v>1</v>
       </c>
       <c r="F171" s="9">
-        <v>7703039364</v>
+        <v>7703039363</v>
       </c>
       <c r="G171" s="17"/>
       <c r="H171" s="17"/>
       <c r="I171" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J171" s="4" t="s">
         <v>44</v>
@@ -2347,7 +2313,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>1</v>
       </c>
@@ -2362,12 +2328,12 @@
         <v>1</v>
       </c>
       <c r="F172" s="9">
-        <v>7703039365</v>
+        <v>7703039364</v>
       </c>
       <c r="G172" s="17"/>
       <c r="H172" s="17"/>
       <c r="I172" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J172" s="4" t="s">
         <v>44</v>
@@ -2376,7 +2342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>1</v>
       </c>
@@ -2391,12 +2357,12 @@
         <v>1</v>
       </c>
       <c r="F173" s="9">
-        <v>7703039366</v>
+        <v>7703039365</v>
       </c>
       <c r="G173" s="17"/>
       <c r="H173" s="17"/>
       <c r="I173" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J173" s="4" t="s">
         <v>44</v>
@@ -2405,7 +2371,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>1</v>
       </c>
@@ -2420,12 +2386,12 @@
         <v>1</v>
       </c>
       <c r="F174" s="9">
-        <v>7703039367</v>
+        <v>7703039366</v>
       </c>
       <c r="G174" s="17"/>
       <c r="H174" s="17"/>
       <c r="I174" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J174" s="4" t="s">
         <v>44</v>
@@ -2434,7 +2400,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>1</v>
       </c>
@@ -2449,12 +2415,12 @@
         <v>1</v>
       </c>
       <c r="F175" s="9">
-        <v>7703039368</v>
+        <v>7703039367</v>
       </c>
       <c r="G175" s="17"/>
       <c r="H175" s="17"/>
       <c r="I175" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J175" s="4" t="s">
         <v>44</v>
@@ -2463,48 +2429,48 @@
         <v>45</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B176" s="12"/>
-      <c r="C176" s="12"/>
-      <c r="D176" s="12"/>
-      <c r="E176" s="13"/>
-      <c r="F176" s="11"/>
-      <c r="G176" s="18"/>
-      <c r="H176" s="18"/>
-      <c r="I176" s="12"/>
-      <c r="J176" s="13"/>
-      <c r="K176" s="12"/>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>1</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C238" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D238" s="3"/>
-      <c r="E238" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F238" s="9">
-        <v>7703039429</v>
-      </c>
-      <c r="G238" s="17"/>
-      <c r="H238" s="17"/>
-      <c r="I238" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J238" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K238" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>1</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D176" s="3"/>
+      <c r="E176" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F176" s="9">
+        <v>7703039368</v>
+      </c>
+      <c r="G176" s="17"/>
+      <c r="H176" s="17"/>
+      <c r="I176" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J176" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="177" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B177" s="12"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="11"/>
+      <c r="G177" s="18"/>
+      <c r="H177" s="18"/>
+      <c r="I177" s="12"/>
+      <c r="J177" s="13"/>
+      <c r="K177" s="12"/>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>1</v>
       </c>
@@ -2519,12 +2485,12 @@
         <v>1</v>
       </c>
       <c r="F239" s="9">
-        <v>7703039430</v>
+        <v>7703039429</v>
       </c>
       <c r="G239" s="17"/>
       <c r="H239" s="17"/>
       <c r="I239" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J239" s="4" t="s">
         <v>46</v>
@@ -2533,7 +2499,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>1</v>
       </c>
@@ -2548,12 +2514,12 @@
         <v>1</v>
       </c>
       <c r="F240" s="9">
-        <v>7703039431</v>
+        <v>7703039430</v>
       </c>
       <c r="G240" s="17"/>
       <c r="H240" s="17"/>
       <c r="I240" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J240" s="4" t="s">
         <v>46</v>
@@ -2562,7 +2528,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>1</v>
       </c>
@@ -2577,12 +2543,12 @@
         <v>1</v>
       </c>
       <c r="F241" s="9">
-        <v>7703039432</v>
+        <v>7703039431</v>
       </c>
       <c r="G241" s="17"/>
       <c r="H241" s="17"/>
       <c r="I241" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J241" s="4" t="s">
         <v>46</v>
@@ -2591,7 +2557,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>1</v>
       </c>
@@ -2606,12 +2572,12 @@
         <v>1</v>
       </c>
       <c r="F242" s="9">
-        <v>7703039433</v>
+        <v>7703039432</v>
       </c>
       <c r="G242" s="17"/>
       <c r="H242" s="17"/>
       <c r="I242" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J242" s="4" t="s">
         <v>46</v>
@@ -2620,7 +2586,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>1</v>
       </c>
@@ -2635,12 +2601,12 @@
         <v>1</v>
       </c>
       <c r="F243" s="9">
-        <v>7703039434</v>
+        <v>7703039433</v>
       </c>
       <c r="G243" s="17"/>
       <c r="H243" s="17"/>
       <c r="I243" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J243" s="4" t="s">
         <v>46</v>
@@ -2649,7 +2615,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>1</v>
       </c>
@@ -2664,12 +2630,12 @@
         <v>1</v>
       </c>
       <c r="F244" s="9">
-        <v>7703039435</v>
+        <v>7703039434</v>
       </c>
       <c r="G244" s="17"/>
       <c r="H244" s="17"/>
       <c r="I244" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J244" s="4" t="s">
         <v>46</v>
@@ -2678,7 +2644,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>1</v>
       </c>
@@ -2693,12 +2659,12 @@
         <v>1</v>
       </c>
       <c r="F245" s="9">
-        <v>7703039436</v>
+        <v>7703039435</v>
       </c>
       <c r="G245" s="17"/>
       <c r="H245" s="17"/>
       <c r="I245" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J245" s="4" t="s">
         <v>46</v>
@@ -2707,7 +2673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>1</v>
       </c>
@@ -2722,12 +2688,12 @@
         <v>1</v>
       </c>
       <c r="F246" s="9">
-        <v>7703039437</v>
+        <v>7703039436</v>
       </c>
       <c r="G246" s="17"/>
       <c r="H246" s="17"/>
       <c r="I246" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J246" s="4" t="s">
         <v>46</v>
@@ -2736,7 +2702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>1</v>
       </c>
@@ -2751,12 +2717,12 @@
         <v>1</v>
       </c>
       <c r="F247" s="9">
-        <v>7703039438</v>
+        <v>7703039437</v>
       </c>
       <c r="G247" s="17"/>
       <c r="H247" s="17"/>
       <c r="I247" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J247" s="4" t="s">
         <v>46</v>
@@ -2765,7 +2731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>1</v>
       </c>
@@ -2780,12 +2746,12 @@
         <v>1</v>
       </c>
       <c r="F248" s="9">
-        <v>7703039439</v>
+        <v>7703039438</v>
       </c>
       <c r="G248" s="17"/>
       <c r="H248" s="17"/>
       <c r="I248" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J248" s="4" t="s">
         <v>46</v>
@@ -2794,7 +2760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>1</v>
       </c>
@@ -2809,12 +2775,12 @@
         <v>1</v>
       </c>
       <c r="F249" s="9">
-        <v>7703039440</v>
+        <v>7703039439</v>
       </c>
       <c r="G249" s="17"/>
       <c r="H249" s="17"/>
       <c r="I249" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J249" s="4" t="s">
         <v>46</v>
@@ -2823,7 +2789,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>1</v>
       </c>
@@ -2838,12 +2804,12 @@
         <v>1</v>
       </c>
       <c r="F250" s="9">
-        <v>7703039441</v>
+        <v>7703039440</v>
       </c>
       <c r="G250" s="17"/>
       <c r="H250" s="17"/>
       <c r="I250" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J250" s="4" t="s">
         <v>46</v>
@@ -2852,7 +2818,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>1</v>
       </c>
@@ -2867,12 +2833,12 @@
         <v>1</v>
       </c>
       <c r="F251" s="9">
-        <v>7703039442</v>
+        <v>7703039441</v>
       </c>
       <c r="G251" s="17"/>
       <c r="H251" s="17"/>
       <c r="I251" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J251" s="4" t="s">
         <v>46</v>
@@ -2881,7 +2847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>1</v>
       </c>
@@ -2896,12 +2862,12 @@
         <v>1</v>
       </c>
       <c r="F252" s="9">
-        <v>7703039443</v>
+        <v>7703039442</v>
       </c>
       <c r="G252" s="17"/>
       <c r="H252" s="17"/>
       <c r="I252" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J252" s="4" t="s">
         <v>46</v>
@@ -2910,7 +2876,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -2925,12 +2891,12 @@
         <v>1</v>
       </c>
       <c r="F253" s="9">
-        <v>7703039444</v>
+        <v>7703039443</v>
       </c>
       <c r="G253" s="17"/>
       <c r="H253" s="17"/>
       <c r="I253" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J253" s="4" t="s">
         <v>46</v>
@@ -2939,7 +2905,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>1</v>
       </c>
@@ -2954,12 +2920,12 @@
         <v>1</v>
       </c>
       <c r="F254" s="9">
-        <v>7703039445</v>
+        <v>7703039444</v>
       </c>
       <c r="G254" s="17"/>
       <c r="H254" s="17"/>
       <c r="I254" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J254" s="4" t="s">
         <v>46</v>
@@ -2968,7 +2934,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>1</v>
       </c>
@@ -2983,12 +2949,12 @@
         <v>1</v>
       </c>
       <c r="F255" s="9">
-        <v>7703039446</v>
+        <v>7703039445</v>
       </c>
       <c r="G255" s="17"/>
       <c r="H255" s="17"/>
       <c r="I255" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J255" s="4" t="s">
         <v>46</v>
@@ -2997,7 +2963,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>1</v>
       </c>
@@ -3012,12 +2978,12 @@
         <v>1</v>
       </c>
       <c r="F256" s="9">
-        <v>7703039447</v>
+        <v>7703039446</v>
       </c>
       <c r="G256" s="17"/>
       <c r="H256" s="17"/>
       <c r="I256" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J256" s="4" t="s">
         <v>46</v>
@@ -3026,7 +2992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>1</v>
       </c>
@@ -3041,12 +3007,12 @@
         <v>1</v>
       </c>
       <c r="F257" s="9">
-        <v>7703039448</v>
+        <v>7703039447</v>
       </c>
       <c r="G257" s="17"/>
       <c r="H257" s="17"/>
       <c r="I257" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J257" s="4" t="s">
         <v>46</v>
@@ -3055,7 +3021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>1</v>
       </c>
@@ -3070,12 +3036,12 @@
         <v>1</v>
       </c>
       <c r="F258" s="9">
-        <v>7703039449</v>
+        <v>7703039448</v>
       </c>
       <c r="G258" s="17"/>
       <c r="H258" s="17"/>
       <c r="I258" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J258" s="4" t="s">
         <v>46</v>
@@ -3084,7 +3050,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -3099,12 +3065,12 @@
         <v>1</v>
       </c>
       <c r="F259" s="9">
-        <v>7703039450</v>
+        <v>7703039449</v>
       </c>
       <c r="G259" s="17"/>
       <c r="H259" s="17"/>
       <c r="I259" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J259" s="4" t="s">
         <v>46</v>
@@ -3113,7 +3079,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>1</v>
       </c>
@@ -3128,12 +3094,12 @@
         <v>1</v>
       </c>
       <c r="F260" s="9">
-        <v>7703039451</v>
+        <v>7703039450</v>
       </c>
       <c r="G260" s="17"/>
       <c r="H260" s="17"/>
       <c r="I260" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J260" s="4" t="s">
         <v>46</v>
@@ -3142,7 +3108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>1</v>
       </c>
@@ -3157,12 +3123,12 @@
         <v>1</v>
       </c>
       <c r="F261" s="9">
-        <v>7703039452</v>
+        <v>7703039451</v>
       </c>
       <c r="G261" s="17"/>
       <c r="H261" s="17"/>
       <c r="I261" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J261" s="4" t="s">
         <v>46</v>
@@ -3171,7 +3137,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>1</v>
       </c>
@@ -3186,12 +3152,12 @@
         <v>1</v>
       </c>
       <c r="F262" s="9">
-        <v>7703039453</v>
+        <v>7703039452</v>
       </c>
       <c r="G262" s="17"/>
       <c r="H262" s="17"/>
       <c r="I262" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J262" s="4" t="s">
         <v>46</v>
@@ -3200,7 +3166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>1</v>
       </c>
@@ -3215,12 +3181,12 @@
         <v>1</v>
       </c>
       <c r="F263" s="9">
-        <v>7703039454</v>
+        <v>7703039453</v>
       </c>
       <c r="G263" s="17"/>
       <c r="H263" s="17"/>
       <c r="I263" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J263" s="4" t="s">
         <v>46</v>
@@ -3229,7 +3195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>1</v>
       </c>
@@ -3244,12 +3210,12 @@
         <v>1</v>
       </c>
       <c r="F264" s="9">
-        <v>7703039455</v>
+        <v>7703039454</v>
       </c>
       <c r="G264" s="17"/>
       <c r="H264" s="17"/>
       <c r="I264" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J264" s="4" t="s">
         <v>46</v>
@@ -3258,7 +3224,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>1</v>
       </c>
@@ -3273,12 +3239,12 @@
         <v>1</v>
       </c>
       <c r="F265" s="9">
-        <v>7703039456</v>
+        <v>7703039455</v>
       </c>
       <c r="G265" s="17"/>
       <c r="H265" s="17"/>
       <c r="I265" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J265" s="4" t="s">
         <v>46</v>
@@ -3287,7 +3253,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>1</v>
       </c>
@@ -3302,12 +3268,12 @@
         <v>1</v>
       </c>
       <c r="F266" s="9">
-        <v>7703039457</v>
+        <v>7703039456</v>
       </c>
       <c r="G266" s="17"/>
       <c r="H266" s="17"/>
       <c r="I266" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J266" s="4" t="s">
         <v>46</v>
@@ -3316,7 +3282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>1</v>
       </c>
@@ -3331,12 +3297,12 @@
         <v>1</v>
       </c>
       <c r="F267" s="9">
-        <v>7703039458</v>
+        <v>7703039457</v>
       </c>
       <c r="G267" s="17"/>
       <c r="H267" s="17"/>
       <c r="I267" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J267" s="4" t="s">
         <v>46</v>
@@ -3345,7 +3311,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>1</v>
       </c>
@@ -3360,12 +3326,12 @@
         <v>1</v>
       </c>
       <c r="F268" s="9">
-        <v>7703039459</v>
+        <v>7703039458</v>
       </c>
       <c r="G268" s="17"/>
       <c r="H268" s="17"/>
       <c r="I268" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J268" s="4" t="s">
         <v>46</v>
@@ -3374,7 +3340,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>1</v>
       </c>
@@ -3389,12 +3355,12 @@
         <v>1</v>
       </c>
       <c r="F269" s="9">
-        <v>7703039460</v>
+        <v>7703039459</v>
       </c>
       <c r="G269" s="17"/>
       <c r="H269" s="17"/>
       <c r="I269" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J269" s="4" t="s">
         <v>46</v>
@@ -3403,7 +3369,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>1</v>
       </c>
@@ -3418,12 +3384,12 @@
         <v>1</v>
       </c>
       <c r="F270" s="9">
-        <v>7703039461</v>
+        <v>7703039460</v>
       </c>
       <c r="G270" s="17"/>
       <c r="H270" s="17"/>
       <c r="I270" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J270" s="4" t="s">
         <v>46</v>
@@ -3432,7 +3398,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>1</v>
       </c>
@@ -3447,12 +3413,12 @@
         <v>1</v>
       </c>
       <c r="F271" s="9">
-        <v>7703039462</v>
+        <v>7703039461</v>
       </c>
       <c r="G271" s="17"/>
       <c r="H271" s="17"/>
       <c r="I271" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J271" s="4" t="s">
         <v>46</v>
@@ -3461,7 +3427,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>1</v>
       </c>
@@ -3476,12 +3442,12 @@
         <v>1</v>
       </c>
       <c r="F272" s="9">
-        <v>7703039463</v>
+        <v>7703039462</v>
       </c>
       <c r="G272" s="17"/>
       <c r="H272" s="17"/>
       <c r="I272" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J272" s="4" t="s">
         <v>46</v>
@@ -3490,7 +3456,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>1</v>
       </c>
@@ -3505,12 +3471,12 @@
         <v>1</v>
       </c>
       <c r="F273" s="9">
-        <v>7703039464</v>
+        <v>7703039463</v>
       </c>
       <c r="G273" s="17"/>
       <c r="H273" s="17"/>
       <c r="I273" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J273" s="4" t="s">
         <v>46</v>
@@ -3519,7 +3485,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>1</v>
       </c>
@@ -3534,12 +3500,12 @@
         <v>1</v>
       </c>
       <c r="F274" s="9">
-        <v>7703039465</v>
+        <v>7703039464</v>
       </c>
       <c r="G274" s="17"/>
       <c r="H274" s="17"/>
       <c r="I274" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J274" s="4" t="s">
         <v>46</v>
@@ -3548,7 +3514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>1</v>
       </c>
@@ -3563,12 +3529,12 @@
         <v>1</v>
       </c>
       <c r="F275" s="9">
-        <v>7703039466</v>
+        <v>7703039465</v>
       </c>
       <c r="G275" s="17"/>
       <c r="H275" s="17"/>
       <c r="I275" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J275" s="4" t="s">
         <v>46</v>
@@ -3577,7 +3543,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>1</v>
       </c>
@@ -3592,12 +3558,12 @@
         <v>1</v>
       </c>
       <c r="F276" s="9">
-        <v>7703039467</v>
+        <v>7703039466</v>
       </c>
       <c r="G276" s="17"/>
       <c r="H276" s="17"/>
       <c r="I276" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J276" s="4" t="s">
         <v>46</v>
@@ -3606,32 +3572,61 @@
         <v>47</v>
       </c>
     </row>
-    <row r="277" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>1</v>
       </c>
-      <c r="B277" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C277" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D277" s="5"/>
-      <c r="E277" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F277" s="10">
+      <c r="B277" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D277" s="3"/>
+      <c r="E277" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F277" s="9">
+        <v>7703039467</v>
+      </c>
+      <c r="G277" s="17"/>
+      <c r="H277" s="17"/>
+      <c r="I277" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J277" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K277" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>1</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D278" s="5"/>
+      <c r="E278" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F278" s="10">
         <v>7703039468</v>
       </c>
-      <c r="G277" s="19"/>
-      <c r="H277" s="19"/>
-      <c r="I277" s="5" t="s">
+      <c r="G278" s="19"/>
+      <c r="H278" s="19"/>
+      <c r="I278" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="J277" s="6" t="s">
+      <c r="J278" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K277" s="5" t="s">
+      <c r="K278" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3646,6 +3641,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A638DD4EB1C1A84A89FFB469BA74ACC8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="51af6b70a4447e92b009e517bae45f5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67252fe7-6b63-4403-af0d-37df51d7c3a2" xmlns:ns3="1a0cd919-d361-40f9-9afc-7bc6ff95d333" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="760a45eaac0c1eb6b3a790365277345f" ns2:_="" ns3:_="">
     <xsd:import namespace="67252fe7-6b63-4403-af0d-37df51d7c3a2"/>
@@ -3840,15 +3844,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3861,6 +3856,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71DB8EA9-1E02-4059-870F-414FF031F625}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3875,14 +3878,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37869A15-A724-4BC9-8EFD-824D3F82BD0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
TEST ISSAM TO TESTOPS
</commit_message>
<xml_diff>
--- a/Data Files/JDD Automatisation.xlsx
+++ b/Data Files/JDD Automatisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISSAM.RHARBAOUI\git\ANEF-RenouvellementSejour\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B56A0EA-C600-49B7-8D09-F1C11FAAACD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20D9ED2-D9B8-41E9-B9D8-F0346F47521E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -891,7 +891,7 @@
   <dimension ref="A1:M226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,7 +974,7 @@
         <v>61</v>
       </c>
       <c r="H2" s="16">
-        <v>7703043876</v>
+        <v>7703043875</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>93</v>

</xml_diff>